<commit_message>
amended test cases and added updated test result + bug metrics
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sychien.2014\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sychien.2014\Documents\GitHub\Ulink\Documentation\Metrics\Bug Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6996" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6996"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
     <sheet name="Mitigation Plan" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>Iter.</t>
+  </si>
+  <si>
+    <t>Client - Create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should show success result </t>
+  </si>
+  <si>
+    <t>solved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screening - CRUD </t>
+  </si>
+  <si>
+    <t>System should show success result / redirect back to screening page</t>
+  </si>
+  <si>
+    <t>Unable to edit any screenings</t>
   </si>
 </sst>
 </file>
@@ -189,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -249,11 +267,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,6 +307,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,8 +327,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -686,17 +732,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9">
+      <c r="A2" s="14">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
@@ -705,14 +751,14 @@
         <v>29</v>
       </c>
       <c r="G2" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="9"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
@@ -736,12 +782,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="8">
         <v>1</v>
@@ -760,7 +806,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="9"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -784,7 +830,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -807,27 +853,75 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="14"/>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="14"/>
+      <c r="B8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="19">
+        <v>6</v>
+      </c>
+      <c r="D8" s="20">
+        <v>4</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="11">
+        <v>9</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13">
-        <f>SUM(G2:G6)</f>
-        <v>30</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="10">
+        <f>SUM(G2:G7)</f>
+        <v>31</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -835,10 +929,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -851,9 +945,10 @@
     <col min="6" max="6" width="14.20703125" customWidth="1"/>
     <col min="8" max="8" width="6.41796875" customWidth="1"/>
     <col min="10" max="10" width="10.83984375" customWidth="1"/>
+    <col min="11" max="11" width="10.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -917,12 +1012,14 @@
         <v>1</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J2" s="7">
         <v>42673</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="7">
+        <v>42674</v>
+      </c>
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -951,12 +1048,14 @@
         <v>5</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J3" s="7">
         <v>42673</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="7">
+        <v>42674</v>
+      </c>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -985,46 +1084,50 @@
         <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J4" s="7">
         <v>42673</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="7">
+        <v>42674</v>
+      </c>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="6">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J5" s="7">
         <v>42673</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="7">
+        <v>42674</v>
+      </c>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1038,7 +1141,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>17</v>
@@ -1053,12 +1156,14 @@
         <v>5</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J6" s="7">
         <v>42673</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="7">
+        <v>42674</v>
+      </c>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1072,27 +1177,29 @@
         <v>12</v>
       </c>
       <c r="D7" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J7" s="7">
         <v>42673</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="7">
+        <v>42674</v>
+      </c>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1103,10 +1210,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>17</v>
@@ -1121,12 +1228,14 @@
         <v>1</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J8" s="7">
         <v>42673</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="7">
+        <v>42674</v>
+      </c>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1137,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1146,21 +1255,23 @@
         <v>17</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J9" s="7">
         <v>42673</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="7">
+        <v>42674</v>
+      </c>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1171,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1189,38 +1300,40 @@
         <v>5</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J10" s="7">
         <v>42673</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="7">
+        <v>42674</v>
+      </c>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="13">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="13">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="6">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>32</v>
@@ -1230,6 +1343,210 @@
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="13">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="7">
+        <v>42673</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="7">
+        <v>42673</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="13">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="7">
+        <v>42673</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="13">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="7">
+        <v>42673</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="13">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="7">
+        <v>42673</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="13">
+        <v>2</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="13">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="13">
+        <v>5</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="7">
+        <v>42673</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the score for bug metrics
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6996"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
@@ -315,6 +315,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -326,15 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -732,7 +732,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="14">
+      <c r="A2" s="17">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -758,7 +758,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="14"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
@@ -782,7 +782,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="14"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -806,7 +806,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="14"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -830,7 +830,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -854,7 +854,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="14"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
@@ -878,17 +878,17 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="15">
         <v>6</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="16">
         <v>4</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="16">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -902,17 +902,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="10">
-        <f>SUM(G2:G7)</f>
-        <v>31</v>
+        <f>SUM(G2:G8)</f>
+        <v>40</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>33</v>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1264,14 +1264,12 @@
         <v>5</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J9" s="7">
         <v>42673</v>
       </c>
-      <c r="K9" s="7">
-        <v>42674</v>
-      </c>
+      <c r="K9" s="7"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1300,14 +1298,12 @@
         <v>5</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J10" s="7">
         <v>42673</v>
       </c>
-      <c r="K10" s="7">
-        <v>42674</v>
-      </c>
+      <c r="K10" s="7"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Update bug log + test result
- [client] create client resolved.
- [timeline] illness cannot be added (used to be able to add for
individuals but now cannot for individuals and all)
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Unable to edit any screenings</t>
+  </si>
+  <si>
+    <t>Unable to add / no display</t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -931,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -942,7 +945,7 @@
     <col min="3" max="3" width="17.1015625" customWidth="1"/>
     <col min="4" max="4" width="5.05078125" customWidth="1"/>
     <col min="5" max="5" width="21.68359375" customWidth="1"/>
-    <col min="6" max="6" width="14.20703125" customWidth="1"/>
+    <col min="6" max="6" width="23.62890625" customWidth="1"/>
     <col min="8" max="8" width="6.41796875" customWidth="1"/>
     <col min="10" max="10" width="10.83984375" customWidth="1"/>
     <col min="11" max="11" width="10.15625" bestFit="1" customWidth="1"/>
@@ -1332,12 +1335,14 @@
         <v>1</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J11" s="7">
         <v>42673</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="7">
+        <v>42675</v>
+      </c>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1366,12 +1371,14 @@
         <v>1</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J12" s="7">
         <v>42673</v>
       </c>
-      <c r="K12" s="6"/>
+      <c r="K12" s="7">
+        <v>42675</v>
+      </c>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1391,7 +1398,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>26</v>
@@ -1425,7 +1432,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>26</v>
@@ -1459,7 +1466,7 @@
         <v>41</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>26</v>
@@ -1493,7 +1500,7 @@
         <v>41</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
update bug log and testing
1) changed test result for gender and age base on client, consulation
and  referrabl table. final value from the sql still don't tally for the
screen hsot u toke?
2) CRUD for illness, all test cases fail
3) test cases for KPI indo not done yet and values is 0 according aws.
4) kpi for vedors. She still deciding imo.
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP-GIT\Ulink\Documentation\Metrics\Bug Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sychien.2014\Documents\GitHub\Ulink\Documentation\Metrics\Bug Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7002" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Stop current development immediately and resolve bugs. PM to reschedule the project</t>
+  </si>
+  <si>
+    <t>Unable to delete any screenings</t>
   </si>
 </sst>
 </file>
@@ -349,6 +352,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,12 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,40 +738,40 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.62890625" customWidth="1"/>
+    <col min="3" max="3" width="10.5234375" customWidth="1"/>
+    <col min="8" max="8" width="18.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="5.05" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -784,8 +787,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="19">
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -812,8 +815,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="17"/>
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -838,8 +841,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="17"/>
       <c r="B5" s="13" t="s">
         <v>13</v>
       </c>
@@ -864,8 +867,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="17"/>
       <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
@@ -890,8 +893,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="17"/>
       <c r="B7" s="13" t="s">
         <v>15</v>
       </c>
@@ -916,8 +919,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="17"/>
       <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
@@ -942,8 +945,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="17"/>
       <c r="B9" s="14" t="s">
         <v>38</v>
       </c>
@@ -969,15 +972,15 @@
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="15">
         <f>SUM(G3:G9)</f>
         <v>15</v>
@@ -1000,24 +1003,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
-    <col min="4" max="4" width="5.08984375" customWidth="1"/>
-    <col min="5" max="5" width="21.6328125" customWidth="1"/>
-    <col min="6" max="6" width="27.36328125" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.3671875" customWidth="1"/>
+    <col min="3" max="3" width="17.1015625" customWidth="1"/>
+    <col min="4" max="4" width="5.1015625" customWidth="1"/>
+    <col min="5" max="5" width="21.62890625" customWidth="1"/>
+    <col min="6" max="6" width="27.3671875" customWidth="1"/>
+    <col min="8" max="8" width="6.47265625" customWidth="1"/>
+    <col min="10" max="10" width="10.7890625" customWidth="1"/>
+    <col min="11" max="11" width="13.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="35.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1091,7 +1094,7 @@
       </c>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1127,7 +1130,7 @@
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1163,7 +1166,7 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1199,7 +1202,7 @@
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1235,7 +1238,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1271,7 +1274,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1307,7 +1310,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1341,7 +1344,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1375,7 +1378,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1447,7 +1450,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1481,7 +1484,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1515,7 +1518,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1549,7 +1552,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1580,10 +1583,9 @@
       <c r="J16" s="6">
         <v>42673</v>
       </c>
-      <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1617,8 +1619,22 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I18" s="8"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="6">
+        <v>42676</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I26">
@@ -1638,9 +1654,9 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="14" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="12:13" x14ac:dyDescent="0.55000000000000004">
       <c r="L14">
         <v>0</v>
       </c>
@@ -1648,7 +1664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="12:13" x14ac:dyDescent="0.55000000000000004">
       <c r="L15">
         <v>11</v>
       </c>
@@ -1656,7 +1672,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="12:13" x14ac:dyDescent="0.55000000000000004">
       <c r="L16">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
update bug log for gender and age
total count is correct but in wrong age category (all age inflat by 10
years)
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Screening - CRUD (Type Infant)</t>
+  </si>
+  <si>
+    <t>Wrong Output  - output in wrong age category</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1037,7 +1040,7 @@
     <col min="3" max="3" width="30.9453125" customWidth="1"/>
     <col min="4" max="4" width="5.1015625" customWidth="1"/>
     <col min="5" max="5" width="21.62890625" customWidth="1"/>
-    <col min="6" max="6" width="27.3671875" customWidth="1"/>
+    <col min="6" max="6" width="37.83984375" customWidth="1"/>
     <col min="8" max="8" width="6.47265625" customWidth="1"/>
     <col min="10" max="10" width="10.7890625" customWidth="1"/>
     <col min="11" max="11" width="13.7890625" customWidth="1"/>
@@ -1384,7 +1387,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update test cases for login and screenings
- includes part of testing result for login
- updated iter 3 test cases since not doing regression
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sychien.2014\Documents\GitHub\Ulink\Documentation\Metrics\Bug Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smu/Desktop/Ulink/Documentation/Metrics/Bug Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7002" activeTab="1"/>
+    <workbookView xWindow="1780" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
     <sheet name="Mitigation Plan" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -104,9 +110,6 @@
     <t>Fix during buffer time</t>
   </si>
   <si>
-    <t>Fix during planned debugging time</t>
-  </si>
-  <si>
     <t>unsolve</t>
   </si>
   <si>
@@ -150,12 +153,33 @@
   </si>
   <si>
     <t xml:space="preserve">System should show the updated info for screening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>Account Management</t>
+  </si>
+  <si>
+    <t>Total Score for Iteration 3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function dropped </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -  </t>
+  </si>
+  <si>
+    <t>Pushed to future iteration due to rescope</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +249,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -258,7 +288,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -269,7 +299,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -290,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -334,6 +364,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,6 +380,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -719,22 +761,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.62890625" customWidth="1"/>
-    <col min="3" max="3" width="10.5234375" customWidth="1"/>
-    <col min="8" max="8" width="18.15625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -758,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -774,8 +816,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="16">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -798,11 +840,11 @@
         <v>0</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="16"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="19"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -823,11 +865,11 @@
         <v>0</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="16"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -848,13 +890,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="16"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
       <c r="B6" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="15">
         <v>3</v>
@@ -863,10 +905,12 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="16"/>
+      <c r="H6" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="19"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -885,17 +929,16 @@
         <v>0</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="16"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="10">
-        <f t="shared" ref="C8:C10" si="1">SUM(D8:F8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -909,13 +952,13 @@
         <v>0</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="16"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="19"/>
       <c r="B9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
@@ -937,10 +980,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="19"/>
       <c r="B10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10">
         <v>6</v>
@@ -961,15 +1004,15 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
+    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -979,10 +1022,54 @@
         <v>Fix during buffer time</v>
       </c>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>3</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="18">
+        <v>10</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="18">
+        <v>8</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -997,29 +1084,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.7890625" customWidth="1"/>
-    <col min="3" max="3" width="17.1015625" customWidth="1"/>
-    <col min="4" max="4" width="5.1015625" customWidth="1"/>
-    <col min="5" max="5" width="46.9453125" customWidth="1"/>
-    <col min="6" max="6" width="37.83984375" customWidth="1"/>
-    <col min="8" max="8" width="6.47265625" customWidth="1"/>
-    <col min="10" max="10" width="10.7890625" customWidth="1"/>
-    <col min="11" max="11" width="13.7890625" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="37.83203125" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="35.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -1052,7 +1140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1060,16 +1148,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="7">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>23</v>
@@ -1078,15 +1166,19 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="5">
         <v>42673</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1094,16 +1186,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="7">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>23</v>
@@ -1112,13 +1204,17 @@
         <v>5</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="5">
         <v>42673</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:I12 I2:I3">
@@ -1138,9 +1234,9 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="14" spans="12:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L14">
         <v>0</v>
       </c>
@@ -1148,20 +1244,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L15">
         <v>11</v>
       </c>
       <c r="M15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L16">
         <v>21</v>
       </c>
       <c r="M16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update iter 3 test result and bug log & metrics
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smu/Desktop/Ulink/Documentation/Metrics/Bug Metrics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shu Yan\Desktop\Ulink\Documentation\Metrics\Bug Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,23 +16,23 @@
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
     <sheet name="Mitigation Plan" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Task</t>
   </si>
@@ -174,12 +174,111 @@
   </si>
   <si>
     <t>Pushed to future iteration due to rescope</t>
+  </si>
+  <si>
+    <t>Protect</t>
+  </si>
+  <si>
+    <t>Error Message Shown for wrong credentials</t>
+  </si>
+  <si>
+    <t>1,5,8</t>
+  </si>
+  <si>
+    <t>Account created or related message should show</t>
+  </si>
+  <si>
+    <t>No such message, page did not redirect</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Able to change user/admin's password</t>
+  </si>
+  <si>
+    <t>Page did not redirect to anywhere to update password</t>
+  </si>
+  <si>
+    <t>able to login with old password, related to test no 11</t>
+  </si>
+  <si>
+    <t>Redirect to homepage</t>
+  </si>
+  <si>
+    <t>Did not redirect to home page, related to test no 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No error message, not sure is UI not display properly or codes did not do validation for wrong credentials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High </t>
+  </si>
+  <si>
+    <t>Account deleted or related message should show</t>
+  </si>
+  <si>
+    <t>Did not show success message, page did not redirect / refresh. Have to manually refresh to see it work.</t>
+  </si>
+  <si>
+    <t>Did not show success message, page did not redirect / refresh. Have to manually go to acct management page to see it work.</t>
+  </si>
+  <si>
+    <t>15,16</t>
+  </si>
+  <si>
+    <t>Normal user should not able to access the page</t>
+  </si>
+  <si>
+    <t>Can access the page</t>
+  </si>
+  <si>
+    <t>Error Message shown for account existed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No error message. Unsure if the new account overwrites the existing account - checked DB, it did not. </t>
+  </si>
+  <si>
+    <t>20, 21</t>
+  </si>
+  <si>
+    <t>11,22</t>
+  </si>
+  <si>
+    <t>Unable to access the page without login</t>
+  </si>
+  <si>
+    <t>Able to access</t>
+  </si>
+  <si>
+    <t>23,24,25,26</t>
+  </si>
+  <si>
+    <t>18,27</t>
+  </si>
+  <si>
+    <t>Normal user should not have the acct management tab in their header</t>
+  </si>
+  <si>
+    <t>Normal user can view it on the header and can access it</t>
+  </si>
+  <si>
+    <t>Login &amp; Account Management  - login</t>
+  </si>
+  <si>
+    <t>Login &amp; Account Management -acct</t>
+  </si>
+  <si>
+    <t>Login &amp; Account Management -protect</t>
+  </si>
+  <si>
+    <t>Use planned debugging time during iteration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -370,6 +469,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -384,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,7 +543,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -761,20 +872,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
@@ -800,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -816,8 +927,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -843,8 +954,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="20"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -868,8 +979,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="20"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -893,8 +1004,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="20"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -909,8 +1020,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -932,8 +1043,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="20"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -955,8 +1066,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="20"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -980,8 +1091,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="20"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1004,15 +1115,15 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20" t="s">
+    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1022,54 +1133,101 @@
         <v>Fix during buffer time</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="23">
+    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="24">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="18">
-        <v>10</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+        <v>12</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="18">
+        <v>3</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="18">
+        <v>15</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="19">
         <v>8</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="20" t="s">
+      <c r="D13" s="19">
+        <v>4</v>
+      </c>
+      <c r="E13" s="19">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="19">
+        <v>9</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="24"/>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="18">
+        <v>7</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="18">
+        <v>3</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="18">
+        <v>15</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="24"/>
+      <c r="B15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="13">
+        <f>SUM(G12:G14)</f>
+        <v>39</v>
+      </c>
+      <c r="H15" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -1082,27 +1240,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="37.83203125" customWidth="1"/>
-    <col min="8" max="8" width="6.5" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37.81640625" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="12" max="12" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="35.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1140,7 +1298,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1178,7 +1336,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1216,8 +1374,338 @@
         <v>46</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="4">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="4">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="4">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="4">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="4">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="4">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I5:I12 I2:I3">
+  <conditionalFormatting sqref="I5:I13 I2:I3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
@@ -1234,9 +1722,9 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="14" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L14">
         <v>0</v>
       </c>
@@ -1244,7 +1732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L15">
         <v>11</v>
       </c>
@@ -1252,7 +1740,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L16">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Update bug log & metric and test result for iter 6 (screenings only)
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
   <si>
     <t>Task</t>
   </si>
@@ -273,6 +273,87 @@
   </si>
   <si>
     <t>Use planned debugging time during iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenings </t>
+  </si>
+  <si>
+    <t>Screenings</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>Add Screenings</t>
+  </si>
+  <si>
+    <t>Page did not display the screenings since db did not capture the data (screenings)</t>
+  </si>
+  <si>
+    <t>DB did not capture the data (screenings)</t>
+  </si>
+  <si>
+    <t>Unable to edit the newly created screenings (related to test 1,2,3,4)</t>
+  </si>
+  <si>
+    <t>Able to click on the delete button, screening removed from db</t>
+  </si>
+  <si>
+    <t>Displayed unrelated data</t>
+  </si>
+  <si>
+    <t>Display screenings' details according to the filter</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>View filtered screening's client list</t>
+  </si>
+  <si>
+    <t>Page did not redirect to view client list page</t>
+  </si>
+  <si>
+    <t>14,15</t>
+  </si>
+  <si>
+    <t>Able to edit screening (edit those that created in test1,2,3,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page should display the newly created screenings / updated screenings </t>
+  </si>
+  <si>
+    <t>Unable to click on the delete button for this screening as it did not appear (related to test 1,2,3,4)</t>
+  </si>
+  <si>
+    <t>No error message shown (UI)</t>
+  </si>
+  <si>
+    <t>5,7,10</t>
+  </si>
+  <si>
+    <t>Screenings - C</t>
+  </si>
+  <si>
+    <t>Screenings - R</t>
+  </si>
+  <si>
+    <t>Screenings - U</t>
+  </si>
+  <si>
+    <t>Screenings - D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infant's Age validation for add screening </t>
+  </si>
+  <si>
+    <t>Screenings - Filter</t>
+  </si>
+  <si>
+    <t>Screenings - Client List</t>
+  </si>
+  <si>
+    <t>Total Score for Iteration 6</t>
   </si>
 </sst>
 </file>
@@ -355,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -415,11 +496,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -475,6 +580,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,8 +601,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -928,13 +1053,13 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="20">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="22">
         <v>3</v>
       </c>
       <c r="D3" s="6">
@@ -955,11 +1080,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="20"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="22">
         <v>3</v>
       </c>
       <c r="D4" s="6">
@@ -980,11 +1105,11 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="20"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="22">
         <v>3</v>
       </c>
       <c r="D5" s="6">
@@ -1005,11 +1130,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="22">
         <v>3</v>
       </c>
       <c r="D6" s="9"/>
@@ -1021,11 +1146,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="20"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="22">
         <v>2</v>
       </c>
       <c r="D7" s="3">
@@ -1044,11 +1169,11 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="20"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="22">
         <v>1</v>
       </c>
       <c r="D8" s="3">
@@ -1067,11 +1192,11 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="20"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="22">
         <v>3</v>
       </c>
       <c r="D9" s="3">
@@ -1092,11 +1217,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="20"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="22">
         <v>6</v>
       </c>
       <c r="D10" s="8"/>
@@ -1116,14 +1241,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1134,7 +1259,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="24">
+      <c r="A12" s="27">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1155,12 +1280,12 @@
       <c r="G12" s="18">
         <v>15</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="24"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1184,50 +1309,91 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
-      <c r="B14" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="21">
         <v>7</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="21">
         <v>3</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="21" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="18">
         <v>15</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
       </c>
       <c r="H15" s="16"/>
     </row>
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="32">
+        <v>6</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="21">
+        <v>15</v>
+      </c>
+      <c r="D16" s="21">
+        <v>4</v>
+      </c>
+      <c r="E16" s="21">
+        <v>3</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="21">
+        <v>19</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="13">
+        <f>SUM(G16)</f>
+        <v>19</v>
+      </c>
+      <c r="H17" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -1240,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1703,6 +1869,223 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>6</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="7">
+        <v>5</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
+        <v>6</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="4">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="4">
+        <v>8</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7">
+        <v>6</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="4">
+        <v>9</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7">
+        <v>6</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="7">
+        <v>5</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="7">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="29"/>
+      <c r="B22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="28"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:I13 I2:I3">

</xml_diff>

<commit_message>
update test case result
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP-GIT\Ulink\Documentation\Metrics\Bug Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shu Yan\Desktop\Ulink\Documentation\Metrics\Bug Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
   <si>
     <t>Task</t>
   </si>
@@ -194,18 +194,9 @@
     <t>Able to change user/admin's password</t>
   </si>
   <si>
-    <t>Page did not redirect to anywhere to update password</t>
-  </si>
-  <si>
-    <t>able to login with old password, related to test no 11</t>
-  </si>
-  <si>
     <t>Redirect to homepage</t>
   </si>
   <si>
-    <t>Did not redirect to home page, related to test no 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">No error message, not sure is UI not display properly or codes did not do validation for wrong credentials </t>
   </si>
   <si>
@@ -227,9 +218,6 @@
     <t>Error Message shown for account existed</t>
   </si>
   <si>
-    <t xml:space="preserve">No error message. Unsure if the new account overwrites the existing account - checked DB, it did not. </t>
-  </si>
-  <si>
     <t>20, 21</t>
   </si>
   <si>
@@ -278,12 +266,6 @@
     <t>Add Screenings</t>
   </si>
   <si>
-    <t>Page did not display the screenings since db did not capture the data (screenings)</t>
-  </si>
-  <si>
-    <t>Unable to edit the newly created screenings (related to test 1,2,3,4)</t>
-  </si>
-  <si>
     <t>Able to click on the delete button, screening removed from db</t>
   </si>
   <si>
@@ -311,9 +293,6 @@
     <t xml:space="preserve">Page should display the newly created screenings / updated screenings </t>
   </si>
   <si>
-    <t>Unable to click on the delete button for this screening as it did not appear (related to test 1,2,3,4)</t>
-  </si>
-  <si>
     <t>No error message shown (UI)</t>
   </si>
   <si>
@@ -383,9 +362,6 @@
     <t>Empty field error msg shown at wrong field</t>
   </si>
   <si>
-    <t>DB capture data not according to demographic</t>
-  </si>
-  <si>
     <t>Edit screenings</t>
   </si>
   <si>
@@ -402,6 +378,33 @@
   </si>
   <si>
     <t>Username is taken displayed even though new</t>
+  </si>
+  <si>
+    <t>Page did not respond when clicking the reset button, browser then appear out of memory</t>
+  </si>
+  <si>
+    <t>Unable to log in with the updated password, ecf from test no 11</t>
+  </si>
+  <si>
+    <t>able to login with old password, ecf from test no 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message shown for one second but disappear after that. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried to create an account and account was created successfully even though there is an error message citing username taken (not in test case) </t>
+  </si>
+  <si>
+    <t>No screenings in the view screening page, unable to delete</t>
+  </si>
+  <si>
+    <t>No screenings in the view screening page, unable to edit</t>
+  </si>
+  <si>
+    <t>no screenings in the view screening page</t>
+  </si>
+  <si>
+    <t>page refreshed when clicking the add button, but screenings was not added to db.</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -649,6 +652,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -667,25 +681,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1069,14 +1090,14 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
@@ -1102,7 +1123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1118,8 +1139,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="32">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1145,8 +1166,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="32"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1170,8 +1191,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="32"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1195,8 +1216,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="32"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -1211,8 +1232,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="32"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1234,8 +1255,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="32"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1257,8 +1278,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="32"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1282,8 +1303,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="32"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1306,15 +1327,15 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1324,8 +1345,8 @@
         <v>Fix during buffer time</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
+    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="36">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1347,11 +1368,11 @@
         <v>15</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="36"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1374,8 +1395,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="36"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
       </c>
@@ -1395,30 +1416,30 @@
         <v>15</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="36"/>
+      <c r="B15" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
       </c>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="37">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C16" s="21">
         <v>15</v>
@@ -1434,18 +1455,18 @@
         <v>19</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -1462,7 +1483,7 @@
     <mergeCell ref="A16:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1472,27 +1493,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.54296875" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="12" max="12" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1529,7 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="29" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1530,7 +1551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1546,7 +1567,7 @@
       <c r="E2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="27" t="s">
         <v>38</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1568,7 +1589,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1584,7 +1605,7 @@
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="27" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -1606,7 +1627,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1614,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>49</v>
@@ -1622,8 +1643,8 @@
       <c r="E4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>57</v>
+      <c r="F4" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>23</v>
@@ -1636,7 +1657,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1644,7 +1665,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" s="4">
         <v>7</v>
@@ -1652,8 +1673,8 @@
       <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>103</v>
+      <c r="F5" s="27" t="s">
+        <v>96</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>51</v>
@@ -1666,7 +1687,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1674,16 +1695,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>53</v>
+      <c r="F6" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>23</v>
@@ -1691,16 +1712,14 @@
       <c r="H6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5">
-        <v>42887</v>
-      </c>
+      <c r="I6" s="39"/>
+      <c r="J6" s="5">
+        <v>42917</v>
+      </c>
+      <c r="K6" s="5"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1708,7 +1727,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D7" s="4">
         <v>12</v>
@@ -1716,8 +1735,8 @@
       <c r="E7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>54</v>
+      <c r="F7" s="27" t="s">
+        <v>117</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>23</v>
@@ -1725,16 +1744,14 @@
       <c r="H7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="5">
-        <v>42887</v>
-      </c>
+      <c r="I7" s="39"/>
+      <c r="J7" s="5">
+        <v>42917</v>
+      </c>
+      <c r="K7" s="5"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1742,31 +1759,31 @@
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D8" s="4">
         <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="H8" s="4">
         <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1774,16 +1791,16 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D9" s="4">
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>111</v>
+        <v>56</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>104</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
@@ -1796,7 +1813,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1804,16 +1821,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>112</v>
+      <c r="F10" s="27" t="s">
+        <v>105</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>51</v>
@@ -1821,14 +1838,14 @@
       <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="4"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="5">
+        <v>42917</v>
+      </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1836,16 +1853,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>59</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>23</v>
@@ -1853,14 +1870,14 @@
       <c r="H11" s="4">
         <v>5</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="4"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="5">
+        <v>42917</v>
+      </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1868,16 +1885,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D12" s="4">
         <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>23</v>
@@ -1890,7 +1907,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1898,16 +1915,16 @@
         <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>118</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>51</v>
@@ -1920,118 +1937,113 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H14" s="4">
         <v>5</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7">
-        <v>6</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>27</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="23">
         <v>5</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="5">
+        <v>42917</v>
+      </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>14</v>
       </c>
       <c r="B16" s="7">
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H16" s="7">
-        <v>1</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>104</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="7">
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="4">
-        <v>6</v>
+        <v>89</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>122</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>51</v>
@@ -2039,29 +2051,29 @@
       <c r="H17" s="7">
         <v>1</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="39"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>17</v>
+    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>16</v>
       </c>
       <c r="B18" s="7">
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D18" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>121</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>51</v>
@@ -2069,31 +2081,29 @@
       <c r="H18" s="7">
         <v>1</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="7">
         <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>93</v>
+        <v>77</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>51</v>
@@ -2101,62 +2111,62 @@
       <c r="H19" s="7">
         <v>1</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="39"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>18</v>
       </c>
       <c r="B20" s="7">
         <v>6</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="4">
+        <v>9</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>84</v>
-      </c>
       <c r="G20" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H20" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="7">
         <v>6</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>88</v>
+        <v>79</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H21" s="7">
         <v>5</v>
@@ -2166,52 +2176,62 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="C23" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="38"/>
-    </row>
-    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="7">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="23"/>
+      <c r="C24" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="38"/>
+    </row>
+    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>109</v>
+        <v>100</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -2220,14 +2240,18 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="34" t="s">
-        <v>122</v>
+      <c r="E26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2236,13 +2260,15 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="28" t="s">
+        <v>114</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -2250,16 +2276,12 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -2268,13 +2290,15 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -2284,13 +2308,13 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2300,15 +2324,13 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2318,13 +2340,15 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="33" t="s">
-        <v>119</v>
+      <c r="E32" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2334,11 +2358,37 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
+    <row r="33" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
-  <conditionalFormatting sqref="I5:I13 I2:I3">
+  <conditionalFormatting sqref="I2:I3 I5:I13">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
@@ -2356,9 +2406,9 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="14" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L14">
         <v>0</v>
       </c>
@@ -2366,7 +2416,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L15">
         <v>11</v>
       </c>
@@ -2374,7 +2424,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L16">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
test result for login, upload, screenings
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="153">
   <si>
     <t>Task</t>
   </si>
@@ -269,36 +269,18 @@
     <t>Able to click on the delete button, screening removed from db</t>
   </si>
   <si>
-    <t>Displayed unrelated data</t>
-  </si>
-  <si>
     <t>Display screenings' details according to the filter</t>
   </si>
   <si>
-    <t>11,12,13</t>
-  </si>
-  <si>
     <t>View filtered screening's client list</t>
   </si>
   <si>
     <t>Page did not redirect to view client list page</t>
   </si>
   <si>
-    <t>14,15</t>
-  </si>
-  <si>
     <t>Able to edit screening (edit those that created in test1,2,3,4)</t>
   </si>
   <si>
-    <t xml:space="preserve">Page should display the newly created screenings / updated screenings </t>
-  </si>
-  <si>
-    <t>No error message shown (UI)</t>
-  </si>
-  <si>
-    <t>5,7,10</t>
-  </si>
-  <si>
     <t>Screenings - C</t>
   </si>
   <si>
@@ -323,9 +305,6 @@
     <t>Total Score for Iteration 6</t>
   </si>
   <si>
-    <t>Success msg doesn’t show long enough and msg is red</t>
-  </si>
-  <si>
     <t>Solved</t>
   </si>
   <si>
@@ -395,16 +374,140 @@
     <t xml:space="preserve">tried to create an account and account was created successfully even though there is an error message citing username taken (not in test case) </t>
   </si>
   <si>
-    <t>No screenings in the view screening page, unable to delete</t>
-  </si>
-  <si>
     <t>No screenings in the view screening page, unable to edit</t>
   </si>
   <si>
-    <t>no screenings in the view screening page</t>
-  </si>
-  <si>
     <t>page refreshed when clicking the add button, but screenings was not added to db.</t>
+  </si>
+  <si>
+    <t>Success message should show to indicate screenings updated</t>
+  </si>
+  <si>
+    <t>no success message</t>
+  </si>
+  <si>
+    <t>Demograhics affected was updated wrongly</t>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
+    <t>No error message shown (UI), screenings was added</t>
+  </si>
+  <si>
+    <t>Able to filter screenings for infant between 0 to 2 years old</t>
+  </si>
+  <si>
+    <t>Unable to input 0, error message shown was value greater than or equal to 1</t>
+  </si>
+  <si>
+    <t>13,14</t>
+  </si>
+  <si>
+    <t>Displayed all screenings</t>
+  </si>
+  <si>
+    <t>Screenings - sort</t>
+  </si>
+  <si>
+    <t>23-27</t>
+  </si>
+  <si>
+    <t>Display result in a sorted order (asc - desc / desc - asc)</t>
+  </si>
+  <si>
+    <t>Unable to click on the header to sort</t>
+  </si>
+  <si>
+    <t>Screenings - value specific validation</t>
+  </si>
+  <si>
+    <t>Username is taken was shown instead of account created and it appeared for 1 second</t>
+  </si>
+  <si>
+    <t>Login &amp; Account Management - value validation</t>
+  </si>
+  <si>
+    <t>input empty fields should display when clicking the reset password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing happens </t>
+  </si>
+  <si>
+    <t>Redirect to upload page with no error / success message, timestamp updated</t>
+  </si>
+  <si>
+    <t>Error with file or related message should show, timestamp should not be updated</t>
+  </si>
+  <si>
+    <t>Upload - wrong file format</t>
+  </si>
+  <si>
+    <t>Wrong File format shown
+Content should not be found in database 
+Timestamp should not be updated</t>
+  </si>
+  <si>
+    <t>Blank Page</t>
+  </si>
+  <si>
+    <t>Hgh</t>
+  </si>
+  <si>
+    <t>"File successfully updated" shown
+100 Records loaded into database
+Timestamp updated to current time</t>
+  </si>
+  <si>
+    <t>Success message not shown except for 'd', only 99 records loaded in db</t>
+  </si>
+  <si>
+    <t>Success message not shown except for '?', only 294 records loaded in db</t>
+  </si>
+  <si>
+    <t>"File successfully updated" shown
+200 Records loaded into database
+Timestamp updated to current time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"File successfully updated" shown
+300 Records loaded into database
+Timestamp updated to current time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"File successfully updated" shown
+400 Records loaded into database
+Timestamp updated to current time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"File successfully updated" shown
+1000 Records loaded into database
+Row 2003 - 2005 should not be found in database
+Timestamp updated to current time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"File successfully updated" shown
+700 Records loaded into database 
+Row 703 - 705 should not be found in database
+Timestamp updated to current time </t>
+  </si>
+  <si>
+    <t>Success message not shown except for '?', only 392 records loaded in db</t>
+  </si>
+  <si>
+    <t>Success message not shown except for '?', only 985 records loaded in db</t>
+  </si>
+  <si>
+    <t>Success message not shown except for '?', only 689 records loaded in db</t>
+  </si>
+  <si>
+    <t>Upload - correct file format</t>
+  </si>
+  <si>
+    <t>Upload - csv file</t>
+  </si>
+  <si>
+    <t>Upload - wrong header structure, file correct format</t>
   </si>
 </sst>
 </file>
@@ -580,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -663,30 +766,44 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,7 +1257,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="32">
+      <c r="A3" s="34">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1167,7 +1284,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1309,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="32"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1217,7 +1334,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -1233,7 +1350,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1373,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="32"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1279,7 +1396,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1304,7 +1421,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1328,14 +1445,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1346,7 +1463,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="36">
+      <c r="A12" s="38">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1372,7 +1489,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="36"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1396,7 +1513,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="36"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
       </c>
@@ -1420,14 +1537,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="36"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -1435,7 +1552,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="37">
+      <c r="A16" s="39">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1459,14 +1576,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -1493,11 +1610,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1657,7 +1772,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1674,7 +1789,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>51</v>
@@ -1704,7 +1819,7 @@
         <v>52</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>23</v>
@@ -1712,7 +1827,7 @@
       <c r="H6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="5">
         <v>42917</v>
       </c>
@@ -1736,7 +1851,7 @@
         <v>48</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>23</v>
@@ -1744,7 +1859,7 @@
       <c r="H7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="39"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="5">
         <v>42917</v>
       </c>
@@ -1768,7 +1883,7 @@
         <v>53</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>55</v>
@@ -1777,7 +1892,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1800,7 +1915,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
@@ -1830,7 +1945,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>51</v>
@@ -1838,7 +1953,7 @@
       <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="39"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="5">
         <v>42917</v>
       </c>
@@ -1870,7 +1985,7 @@
       <c r="H11" s="4">
         <v>5</v>
       </c>
-      <c r="I11" s="39"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="5">
         <v>42917</v>
       </c>
@@ -1908,7 +2023,7 @@
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="4">
@@ -1924,7 +2039,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>51</v>
@@ -1938,8 +2053,12 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>71</v>
       </c>
@@ -1959,16 +2078,14 @@
         <v>5</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
-        <v>13</v>
-      </c>
+      <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>3</v>
       </c>
@@ -1981,8 +2098,8 @@
       <c r="E15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>119</v>
+      <c r="F15" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>23</v>
@@ -1996,37 +2113,38 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="7">
-        <v>6</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="7">
-        <v>5</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="B16" s="23">
+        <v>3</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16">
+        <v>28</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="23">
+        <v>1</v>
+      </c>
+      <c r="J16" s="43">
+        <v>42948</v>
+      </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2034,46 +2152,48 @@
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H17" s="7">
-        <v>1</v>
-      </c>
-      <c r="I17" s="39"/>
+        <v>5</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
         <v>16</v>
       </c>
       <c r="B18" s="7">
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>51</v>
@@ -2081,29 +2201,29 @@
       <c r="H18" s="7">
         <v>1</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="7">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="7">
         <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D19" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>51</v>
@@ -2111,7 +2231,9 @@
       <c r="H19" s="7">
         <v>1</v>
       </c>
-      <c r="I19" s="39"/>
+      <c r="I19" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -2124,46 +2246,48 @@
         <v>6</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D20" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H20" s="7">
-        <v>1</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="I20" s="32"/>
+      <c r="J20" s="5">
+        <v>42948</v>
+      </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
         <v>19</v>
       </c>
       <c r="B21" s="7">
         <v>6</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>55</v>
@@ -2176,7 +2300,7 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2184,105 +2308,149 @@
         <v>6</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="D22" s="4">
+        <v>12</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H22" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="5">
+        <v>42948</v>
+      </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="7">
+        <v>5</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="C24" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="38"/>
-    </row>
-    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7">
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="7">
+        <v>5</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="23">
+        <v>6</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="23">
+        <v>1</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="J25" s="5">
+        <v>42948</v>
+      </c>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="23"/>
+      <c r="C27" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="40"/>
+    </row>
+    <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -2294,13 +2462,15 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>95</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -2308,15 +2478,15 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -2329,9 +2499,7 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -2344,11 +2512,11 @@
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2358,13 +2526,13 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="27" t="s">
-        <v>111</v>
+      <c r="E33" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2374,21 +2542,255 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G39" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="F42" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" t="s">
+        <v>55</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="G43" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44">
+        <v>9</v>
+      </c>
+      <c r="E44" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G44" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="G45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46">
+        <v>11</v>
+      </c>
+      <c r="E46" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="F46" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" t="s">
+        <v>55</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I3 I5:I13">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+  <conditionalFormatting sqref="I18">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
+  <conditionalFormatting sqref="I20">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update test result for iter 3
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
+    <workbookView minimized="1" xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
   <si>
     <t>Task</t>
   </si>
@@ -457,12 +457,6 @@
     <t>"File successfully updated" shown
 100 Records loaded into database
 Timestamp updated to current time</t>
-  </si>
-  <si>
-    <t>Success message not shown except for 'd', only 99 records loaded in db</t>
-  </si>
-  <si>
-    <t>Success message not shown except for '?', only 294 records loaded in db</t>
   </si>
   <si>
     <t>"File successfully updated" shown
@@ -517,6 +511,25 @@
   </si>
   <si>
     <t>Page redirect to viewscreening page and screenings updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success message not shown except for 'd', only 99 records loaded in db
+db: Clientname So Mang Yang (line 91 not loaded) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success message not shown except for 'd', only 199 records loaded in db
+db: Clientname Johanes Bundjamin (line 16 not loaded) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">not in testcase </t>
+  </si>
+  <si>
+    <t>Upload Testing2.1
+200 records loaded into db</t>
+  </si>
+  <si>
+    <t>Success message not shown except for '?', only 294 records loaded in db
+db: Vicheet Roth (line 193) ,  Edward Supit (line 247), Li You Tan (line 251) , Ry Vanna (line 261),  Khov Seang Ngun (line 295), Tan Lyly (line 298)</t>
   </si>
 </sst>
 </file>
@@ -1618,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2442,16 +2455,16 @@
         <v>6</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D26">
         <v>29</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>23</v>
@@ -2655,7 +2668,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -2673,12 +2686,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D41">
         <v>6</v>
@@ -2687,7 +2700,7 @@
         <v>139</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="G41" t="s">
         <v>55</v>
@@ -2701,13 +2714,13 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D42">
         <v>7</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F42" s="38" t="s">
         <v>137</v>
@@ -2719,21 +2732,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D43">
         <v>8</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="G43" t="s">
         <v>55</v>
@@ -2747,16 +2760,16 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D44">
         <v>9</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G44" t="s">
         <v>55</v>
@@ -2770,16 +2783,16 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D45">
         <v>10</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G45" t="s">
         <v>55</v>
@@ -2793,22 +2806,33 @@
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D46">
         <v>11</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G46" t="s">
         <v>55</v>
       </c>
       <c r="H46">
         <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="D47" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="F47" s="38" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test result and bug log for login, acct management, screenings
data management and client test result and bug log not updated
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="155">
   <si>
     <t>Task</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Normal user should not able to access the page</t>
   </si>
   <si>
-    <t>Can access the page</t>
-  </si>
-  <si>
     <t>Error Message shown for account existed</t>
   </si>
   <si>
@@ -233,15 +230,9 @@
     <t>23,24,25,26</t>
   </si>
   <si>
-    <t>18,27</t>
-  </si>
-  <si>
     <t>Normal user should not have the acct management tab in their header</t>
   </si>
   <si>
-    <t>Normal user can view it on the header and can access it</t>
-  </si>
-  <si>
     <t>Login &amp; Account Management  - login</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
     <t>View filtered screening's client list</t>
   </si>
   <si>
-    <t>Page did not redirect to view client list page</t>
-  </si>
-  <si>
     <t>Able to edit screening (edit those that created in test1,2,3,4)</t>
   </si>
   <si>
@@ -323,9 +311,6 @@
     <t>Cannot log in with new password</t>
   </si>
   <si>
-    <t>????</t>
-  </si>
-  <si>
     <t>Did not show success message</t>
   </si>
   <si>
@@ -371,9 +356,6 @@
     <t xml:space="preserve">Error message shown for one second but disappear after that. </t>
   </si>
   <si>
-    <t xml:space="preserve">tried to create an account and account was created successfully even though there is an error message citing username taken (not in test case) </t>
-  </si>
-  <si>
     <t>No screenings in the view screening page, unable to edit</t>
   </si>
   <si>
@@ -398,13 +380,7 @@
     <t>Able to filter screenings for infant between 0 to 2 years old</t>
   </si>
   <si>
-    <t>Unable to input 0, error message shown was value greater than or equal to 1</t>
-  </si>
-  <si>
     <t>13,14</t>
-  </si>
-  <si>
-    <t>Displayed all screenings</t>
   </si>
   <si>
     <t>Screenings - sort</t>
@@ -510,9 +486,6 @@
     <t>Error message to show "input empty fields"</t>
   </si>
   <si>
-    <t>Page redirect to viewscreening page and screenings updated</t>
-  </si>
-  <si>
     <t xml:space="preserve">Success message not shown except for 'd', only 99 records loaded in db
 db: Clientname So Mang Yang (line 91 not loaded) </t>
   </si>
@@ -530,6 +503,21 @@
   <si>
     <t>Success message not shown except for '?', only 294 records loaded in db
 db: Vicheet Roth (line 193) ,  Edward Supit (line 247), Li You Tan (line 251) , Ry Vanna (line 261),  Khov Seang Ngun (line 295), Tan Lyly (line 298)</t>
+  </si>
+  <si>
+    <t>solved</t>
+  </si>
+  <si>
+    <t>able to access the url and did not redirect to home page or show error message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">able to access edituserpassword and createaccount.html, tried to create an account and account created message shown but db did not capture it </t>
+  </si>
+  <si>
+    <t>Filter missing</t>
+  </si>
+  <si>
+    <t>Filter missing, therefore unable to click on generate button</t>
   </si>
 </sst>
 </file>
@@ -705,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -826,11 +814,82 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1506,7 +1565,7 @@
         <v>15</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -1554,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -1577,7 +1636,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C16" s="21">
         <v>15</v>
@@ -1593,13 +1652,13 @@
         <v>19</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="44"/>
       <c r="B17" s="44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="44"/>
@@ -1621,7 +1680,7 @@
     <mergeCell ref="A16:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1631,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1699,7 +1758,7 @@
       <c r="C2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="46">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1737,7 +1796,7 @@
       <c r="C3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="46">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1773,9 +1832,9 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1803,16 +1862,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="4">
+        <v>67</v>
+      </c>
+      <c r="D5" s="47">
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>51</v>
@@ -1820,7 +1879,9 @@
       <c r="H5" s="4">
         <v>1</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -1833,16 +1894,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>23</v>
@@ -1850,7 +1911,9 @@
       <c r="H6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J6" s="5">
         <v>42917</v>
       </c>
@@ -1865,16 +1928,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="4">
+        <v>66</v>
+      </c>
+      <c r="D7" s="47">
         <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>23</v>
@@ -1882,7 +1945,9 @@
       <c r="H7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J7" s="5">
         <v>42917</v>
       </c>
@@ -1897,16 +1962,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="4">
+        <v>66</v>
+      </c>
+      <c r="D8" s="47">
         <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>55</v>
@@ -1915,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1929,16 +1994,16 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="4">
+        <v>67</v>
+      </c>
+      <c r="D9" s="47">
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
@@ -1946,7 +2011,9 @@
       <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1959,16 +2026,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="47" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>51</v>
@@ -1976,14 +2043,16 @@
       <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J10" s="5">
         <v>42917</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1991,16 +2060,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="D11" s="47">
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>23</v>
@@ -2023,16 +2092,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="4">
+        <v>68</v>
+      </c>
+      <c r="D12" s="47">
         <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>23</v>
@@ -2040,7 +2109,7 @@
       <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="31"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -2053,16 +2122,16 @@
         <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>60</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>51</v>
@@ -2070,7 +2139,9 @@
       <c r="H13" s="4">
         <v>1</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -2083,16 +2154,16 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>64</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="27" t="s">
         <v>63</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>64</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>55</v>
@@ -2101,7 +2172,7 @@
         <v>5</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2113,16 +2184,16 @@
         <v>3</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15">
+        <v>67</v>
+      </c>
+      <c r="D15" s="48">
         <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>23</v>
@@ -2130,6 +2201,7 @@
       <c r="H15" s="23">
         <v>5</v>
       </c>
+      <c r="I15" s="31"/>
       <c r="J15" s="5">
         <v>42917</v>
       </c>
@@ -2144,22 +2216,25 @@
         <v>3</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16">
+        <v>122</v>
+      </c>
+      <c r="D16" s="48">
         <v>28</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G16" s="23" t="s">
         <v>51</v>
       </c>
       <c r="H16" s="23">
         <v>1</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="J16" s="35">
         <v>42948</v>
@@ -2175,16 +2250,16 @@
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>72</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>23</v>
@@ -2193,7 +2268,7 @@
         <v>5</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2207,16 +2282,16 @@
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="4">
+        <v>79</v>
+      </c>
+      <c r="D18" s="47">
         <v>7</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>51</v>
@@ -2224,7 +2299,9 @@
       <c r="H18" s="7">
         <v>1</v>
       </c>
-      <c r="I18" s="31"/>
+      <c r="I18" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -2237,16 +2314,16 @@
         <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="4">
+        <v>80</v>
+      </c>
+      <c r="D19" s="47">
         <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>51</v>
@@ -2255,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2269,16 +2346,16 @@
         <v>6</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="4">
+        <v>81</v>
+      </c>
+      <c r="D20" s="47">
         <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>23</v>
@@ -2286,7 +2363,9 @@
       <c r="H20" s="7">
         <v>5</v>
       </c>
-      <c r="I20" s="31"/>
+      <c r="I20" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="J20" s="5">
         <v>42948</v>
       </c>
@@ -2301,16 +2380,16 @@
         <v>6</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>112</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>55</v>
@@ -2318,12 +2397,14 @@
       <c r="H21" s="7">
         <v>5</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2331,16 +2412,16 @@
         <v>6</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="4">
+        <v>83</v>
+      </c>
+      <c r="D22" s="47">
         <v>12</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>51</v>
@@ -2348,7 +2429,7 @@
       <c r="H22" s="7">
         <v>1</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="31"/>
       <c r="J22" s="5">
         <v>42948</v>
       </c>
@@ -2363,16 +2444,16 @@
         <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>122</v>
+        <v>83</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>115</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>55</v>
@@ -2380,7 +2461,7 @@
       <c r="H23" s="7">
         <v>5</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -2393,16 +2474,16 @@
         <v>6</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="47" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>23</v>
@@ -2410,7 +2491,7 @@
       <c r="H24" s="7">
         <v>5</v>
       </c>
-      <c r="I24" s="4"/>
+      <c r="I24" s="31"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -2423,16 +2504,16 @@
         <v>6</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>125</v>
+        <v>116</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>117</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>51</v>
@@ -2440,7 +2521,7 @@
       <c r="H25" s="23">
         <v>1</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="5">
         <v>42948</v>
       </c>
@@ -2455,16 +2536,16 @@
         <v>6</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26">
-        <v>29</v>
+        <v>143</v>
+      </c>
+      <c r="D26" s="48">
+        <v>30</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>23</v>
@@ -2472,6 +2553,7 @@
       <c r="H26" s="23">
         <v>5</v>
       </c>
+      <c r="I26" s="31"/>
       <c r="J26" s="5">
         <v>42948</v>
       </c>
@@ -2479,10 +2561,11 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
       <c r="C27" s="30" t="s">
-        <v>92</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D27" s="48"/>
       <c r="E27" s="45" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F27" s="45"/>
     </row>
@@ -2490,18 +2573,20 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="D28" s="47"/>
       <c r="E28" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -2510,18 +2595,20 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -2530,14 +2617,16 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="4"/>
       <c r="F30" s="28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2546,7 +2635,7 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="47"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2560,16 +2649,18 @@
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="D32" s="47"/>
       <c r="E32" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -2578,9 +2669,9 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2594,9 +2685,9 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="47"/>
       <c r="E34" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2610,16 +2701,18 @@
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="D35" s="47"/>
       <c r="E35" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2628,9 +2721,9 @@
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="27" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2640,21 +2733,27 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
     </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D37" s="48"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D38" s="48"/>
+    </row>
     <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" t="s">
-        <v>75</v>
+        <v>127</v>
+      </c>
+      <c r="D39" s="48" t="s">
+        <v>72</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F39" s="36" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G39" t="s">
         <v>51</v>
@@ -2668,19 +2767,19 @@
         <v>7</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="D40">
+        <v>142</v>
+      </c>
+      <c r="D40" s="48">
         <v>5</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G40" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H40">
         <v>5</v>
@@ -2691,16 +2790,16 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41">
+        <v>140</v>
+      </c>
+      <c r="D41" s="48">
         <v>6</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G41" t="s">
         <v>55</v>
@@ -2714,16 +2813,16 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>149</v>
-      </c>
-      <c r="D42">
+        <v>141</v>
+      </c>
+      <c r="D42" s="48">
         <v>7</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G42" t="s">
         <v>55</v>
@@ -2737,16 +2836,16 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>148</v>
-      </c>
-      <c r="D43">
+        <v>140</v>
+      </c>
+      <c r="D43" s="48">
         <v>8</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G43" t="s">
         <v>55</v>
@@ -2760,16 +2859,16 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>148</v>
-      </c>
-      <c r="D44">
+        <v>140</v>
+      </c>
+      <c r="D44" s="48">
         <v>9</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G44" t="s">
         <v>55</v>
@@ -2783,16 +2882,16 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
-      </c>
-      <c r="D45">
+        <v>140</v>
+      </c>
+      <c r="D45" s="48">
         <v>10</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G45" t="s">
         <v>55</v>
@@ -2806,16 +2905,16 @@
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46">
+        <v>140</v>
+      </c>
+      <c r="D46" s="48">
         <v>11</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G46" t="s">
         <v>55</v>
@@ -2825,31 +2924,176 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="D47" s="38" t="s">
-        <v>156</v>
+      <c r="D47" s="50" t="s">
+        <v>147</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>155</v>
-      </c>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D48" s="48"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D49" s="48"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D50" s="48"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D51" s="48"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D52" s="48"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D53" s="48"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D54" s="48"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D55" s="48"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D56" s="48"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D57" s="48"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D58" s="48"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D59" s="48"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D60" s="48"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D61" s="48"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D62" s="48"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D63" s="48"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D64" s="48"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D65" s="48"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D66" s="48"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D67" s="48"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D68" s="48"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D69" s="48"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D70" s="48"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D71" s="48"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D72" s="48"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D73" s="48"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D74" s="48"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D75" s="48"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D76" s="48"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D77" s="48"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D78" s="48"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D79" s="48"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D80" s="48"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D81" s="48"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D82" s="48"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D83" s="48"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D84" s="48"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D85" s="48"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D86" s="48"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D87" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E27:F27"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I3 I5:I13">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"unsolve"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="I25">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+  <conditionalFormatting sqref="I26">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update iter 7 bug metric
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="166">
   <si>
     <t>Task</t>
   </si>
@@ -518,6 +518,39 @@
   </si>
   <si>
     <t>Filter missing, therefore unable to click on generate button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clients Page - Sort Client </t>
+  </si>
+  <si>
+    <t>1 - 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client - Display Profile </t>
+  </si>
+  <si>
+    <t>15 , 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Client's profile </t>
+  </si>
+  <si>
+    <t>Unable to click on client's name to view its profile</t>
+  </si>
+  <si>
+    <t>Sort Clients in an order</t>
+  </si>
+  <si>
+    <t>No cients displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16, 18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">View Client's appointments </t>
+  </si>
+  <si>
+    <t>Unable to view</t>
   </si>
 </sst>
 </file>
@@ -693,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -793,6 +826,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -814,47 +862,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1337,7 +1352,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="39">
+      <c r="A3" s="44">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1364,7 +1379,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1389,7 +1404,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1414,7 +1429,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -1430,7 +1445,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1453,7 +1468,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1476,7 +1491,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="39"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1501,7 +1516,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1525,14 +1540,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
-      <c r="B11" s="40" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1543,7 +1558,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="48">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1569,7 +1584,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="43"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1593,7 +1608,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
       </c>
@@ -1617,14 +1632,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="43"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="48"/>
+      <c r="B15" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -1632,7 +1647,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="44">
+      <c r="A16" s="49">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1656,14 +1671,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="49"/>
+      <c r="B17" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -1680,7 +1695,7 @@
     <mergeCell ref="A16:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1690,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1758,7 +1773,7 @@
       <c r="C2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="39">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1796,7 +1811,7 @@
       <c r="C3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="39">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1834,7 +1849,7 @@
       <c r="C4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="40" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1864,7 +1879,7 @@
       <c r="C5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="40">
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1896,7 +1911,7 @@
       <c r="C6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="40" t="s">
         <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1930,7 +1945,7 @@
       <c r="C7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="40">
         <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1964,7 +1979,7 @@
       <c r="C8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="40">
         <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1996,7 +2011,7 @@
       <c r="C9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="40">
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -2028,7 +2043,7 @@
       <c r="C10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="40" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -2062,7 +2077,7 @@
       <c r="C11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="40">
         <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -2094,7 +2109,7 @@
       <c r="C12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="40">
         <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -2124,7 +2139,7 @@
       <c r="C13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="40" t="s">
         <v>60</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -2156,7 +2171,7 @@
       <c r="C14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="40" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -2186,7 +2201,7 @@
       <c r="C15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="41">
         <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -2218,7 +2233,7 @@
       <c r="C16" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="41">
         <v>28</v>
       </c>
       <c r="E16" s="23" t="s">
@@ -2252,7 +2267,7 @@
       <c r="C17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="39" t="s">
         <v>72</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -2284,7 +2299,7 @@
       <c r="C18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="40">
         <v>7</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -2316,7 +2331,7 @@
       <c r="C19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="40">
         <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -2348,7 +2363,7 @@
       <c r="C20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="40">
         <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -2382,7 +2397,7 @@
       <c r="C21" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="40" t="s">
         <v>112</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -2414,7 +2429,7 @@
       <c r="C22" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="40">
         <v>12</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -2446,7 +2461,7 @@
       <c r="C23" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="40" t="s">
         <v>115</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -2476,7 +2491,7 @@
       <c r="C24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="47" t="s">
+      <c r="D24" s="40" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="7" t="s">
@@ -2506,7 +2521,7 @@
       <c r="C25" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="42" t="s">
         <v>117</v>
       </c>
       <c r="E25" s="23" t="s">
@@ -2538,7 +2553,7 @@
       <c r="C26" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="41">
         <v>30</v>
       </c>
       <c r="E26" s="23" t="s">
@@ -2563,11 +2578,11 @@
       <c r="C27" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="45" t="s">
+      <c r="D27" s="41"/>
+      <c r="E27" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="45"/>
+      <c r="F27" s="50"/>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
@@ -2575,7 +2590,7 @@
       <c r="C28" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="40"/>
       <c r="E28" s="4" t="s">
         <v>89</v>
       </c>
@@ -2597,7 +2612,7 @@
       <c r="C29" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="4" t="s">
         <v>90</v>
       </c>
@@ -2617,7 +2632,7 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="40"/>
       <c r="E30" s="4"/>
       <c r="F30" s="28" t="s">
         <v>102</v>
@@ -2634,13 +2649,19 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="40"/>
+      <c r="E31" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -2648,19 +2669,15 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="47"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>150</v>
-      </c>
+      <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -2669,9 +2686,9 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="40"/>
       <c r="E33" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2684,122 +2701,169 @@
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="47"/>
+      <c r="C34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="40"/>
       <c r="E34" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="4" t="s">
-        <v>98</v>
+      <c r="C35" s="4"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="27" t="s">
+        <v>99</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>150</v>
-      </c>
+      <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D37" s="48"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D38" s="48"/>
-    </row>
-    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="G36" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="41">
+        <v>5</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="41">
+        <v>6</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="48" t="s">
-        <v>72</v>
+        <v>141</v>
+      </c>
+      <c r="D39" s="41">
+        <v>7</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F39" s="36" t="s">
-        <v>125</v>
+        <v>132</v>
+      </c>
+      <c r="F39" s="38" t="s">
+        <v>129</v>
       </c>
       <c r="G39" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>7</v>
       </c>
-      <c r="C40" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="D40" s="48">
-        <v>5</v>
+      <c r="C40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" s="41">
+        <v>8</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="G40" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="H40">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>7</v>
       </c>
       <c r="C41" t="s">
         <v>140</v>
       </c>
-      <c r="D41" s="48">
-        <v>6</v>
+      <c r="D41" s="41">
+        <v>9</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G41" t="s">
         <v>55</v>
@@ -2808,21 +2872,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" s="48">
-        <v>7</v>
+        <v>140</v>
+      </c>
+      <c r="D42" s="41">
+        <v>10</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="G42" t="s">
         <v>55</v>
@@ -2831,21 +2895,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>7</v>
       </c>
       <c r="C43" t="s">
         <v>140</v>
       </c>
-      <c r="D43" s="48">
-        <v>8</v>
+      <c r="D43" s="41">
+        <v>11</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G43" t="s">
         <v>55</v>
@@ -2854,21 +2918,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>7</v>
       </c>
       <c r="C44" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="48">
-        <v>9</v>
+      <c r="D44" s="43" t="s">
+        <v>147</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="G44" t="s">
         <v>55</v>
@@ -2877,21 +2941,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="48">
-        <v>10</v>
+        <v>155</v>
+      </c>
+      <c r="D45" s="51" t="s">
+        <v>156</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="G45" t="s">
         <v>55</v>
@@ -2900,21 +2964,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="48">
-        <v>11</v>
+        <v>157</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="G46" t="s">
         <v>55</v>
@@ -2923,143 +2987,146 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="D47" s="50" t="s">
-        <v>147</v>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="41" t="s">
+        <v>163</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>146</v>
+        <v>165</v>
+      </c>
+      <c r="G47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D48" s="48"/>
+      <c r="D48" s="41"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D49" s="48"/>
+      <c r="D49" s="41"/>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D50" s="48"/>
+      <c r="D50" s="41"/>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D51" s="48"/>
+      <c r="D51" s="41"/>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D52" s="48"/>
+      <c r="D52" s="41"/>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D53" s="48"/>
+      <c r="D53" s="41"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D54" s="48"/>
+      <c r="D54" s="41"/>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D55" s="48"/>
+      <c r="D55" s="41"/>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D56" s="48"/>
+      <c r="D56" s="41"/>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D57" s="48"/>
+      <c r="D57" s="41"/>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D58" s="48"/>
+      <c r="D58" s="41"/>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D59" s="48"/>
+      <c r="D59" s="41"/>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D60" s="48"/>
+      <c r="D60" s="41"/>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D61" s="48"/>
+      <c r="D61" s="41"/>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D62" s="48"/>
+      <c r="D62" s="41"/>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D63" s="48"/>
+      <c r="D63" s="41"/>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D64" s="48"/>
+      <c r="D64" s="41"/>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D65" s="48"/>
+      <c r="D65" s="41"/>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D66" s="48"/>
+      <c r="D66" s="41"/>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D67" s="48"/>
+      <c r="D67" s="41"/>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D68" s="48"/>
+      <c r="D68" s="41"/>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D69" s="48"/>
+      <c r="D69" s="41"/>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D70" s="48"/>
+      <c r="D70" s="41"/>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D71" s="48"/>
+      <c r="D71" s="41"/>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D72" s="48"/>
+      <c r="D72" s="41"/>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D73" s="48"/>
+      <c r="D73" s="41"/>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D74" s="48"/>
+      <c r="D74" s="41"/>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D75" s="48"/>
+      <c r="D75" s="41"/>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D76" s="48"/>
+      <c r="D76" s="41"/>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D77" s="48"/>
+      <c r="D77" s="41"/>
     </row>
     <row r="78" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D78" s="48"/>
+      <c r="D78" s="41"/>
     </row>
     <row r="79" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D79" s="48"/>
+      <c r="D79" s="41"/>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D80" s="48"/>
+      <c r="D80" s="41"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D81" s="48"/>
+      <c r="D81" s="41"/>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D82" s="48"/>
+      <c r="D82" s="41"/>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D83" s="48"/>
+      <c r="D83" s="41"/>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D84" s="48"/>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D85" s="48"/>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D86" s="48"/>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D87" s="48"/>
+      <c r="D84" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E27:F27"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I3 I5:I13">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Clean up data file for bootstrap
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
   <si>
     <t>Task</t>
   </si>
@@ -432,11 +432,6 @@
   <si>
     <t>"File successfully updated" shown
 100 Records loaded into database
-Timestamp updated to current time</t>
-  </si>
-  <si>
-    <t>"File successfully updated" shown
-200 Records loaded into database
 Timestamp updated to current time</t>
   </si>
   <si>
@@ -497,10 +492,6 @@
     <t xml:space="preserve">not in testcase </t>
   </si>
   <si>
-    <t>Upload Testing2.1
-200 records loaded into db</t>
-  </si>
-  <si>
     <t>Success message not shown except for '?', only 294 records loaded in db
 db: Vicheet Roth (line 193) ,  Edward Supit (line 247), Li You Tan (line 251) , Ry Vanna (line 261),  Khov Seang Ngun (line 295), Tan Lyly (line 298)</t>
   </si>
@@ -523,15 +514,9 @@
     <t xml:space="preserve">Clients Page - Sort Client </t>
   </si>
   <si>
-    <t>1 - 14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Client - Display Profile </t>
   </si>
   <si>
-    <t>15 , 17</t>
-  </si>
-  <si>
     <t xml:space="preserve">Display Client's profile </t>
   </si>
   <si>
@@ -544,13 +529,34 @@
     <t>No cients displayed</t>
   </si>
   <si>
-    <t xml:space="preserve">16, 18 </t>
-  </si>
-  <si>
     <t xml:space="preserve">View Client's appointments </t>
   </si>
   <si>
     <t>Unable to view</t>
+  </si>
+  <si>
+    <t>1 - 6</t>
+  </si>
+  <si>
+    <t>7,9</t>
+  </si>
+  <si>
+    <t>8,10</t>
+  </si>
+  <si>
+    <t>"Wrong File Format" shown
+Timestamp should not be updated to current time</t>
+  </si>
+  <si>
+    <t>Upload Testing2.1
+"File successfully updated" shown
+200 records loaded into db, timestamp updated to current time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload - correct file format, wrong header </t>
+  </si>
+  <si>
+    <t>Data not relevant or related message shown</t>
   </si>
 </sst>
 </file>
@@ -841,6 +847,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -860,9 +869,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1352,7 +1358,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="44">
+      <c r="A3" s="45">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1379,7 +1385,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="44"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1404,7 +1410,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="44"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1429,7 +1435,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="44"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -1445,7 +1451,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="44"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1468,7 +1474,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="44"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1491,7 +1497,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="44"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1516,7 +1522,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="44"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1540,14 +1546,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1558,7 +1564,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="48">
+      <c r="A12" s="49">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1584,7 +1590,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="48"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1608,7 +1614,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
       </c>
@@ -1632,14 +1638,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="48"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="49"/>
+      <c r="B15" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="48"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -1647,7 +1653,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="49">
+      <c r="A16" s="50">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1671,14 +1677,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -1705,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47:H47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1895,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1927,7 +1933,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J6" s="5">
         <v>42917</v>
@@ -1961,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J7" s="5">
         <v>42917</v>
@@ -1995,7 +2001,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2027,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2059,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J10" s="5">
         <v>42917</v>
@@ -2084,7 +2090,7 @@
         <v>58</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>23</v>
@@ -2116,7 +2122,7 @@
         <v>65</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>23</v>
@@ -2155,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2208,7 +2214,7 @@
         <v>58</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>23</v>
@@ -2249,7 +2255,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J16" s="35">
         <v>42948</v>
@@ -2436,7 +2442,7 @@
         <v>114</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>51</v>
@@ -2468,7 +2474,7 @@
         <v>75</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>55</v>
@@ -2498,7 +2504,7 @@
         <v>76</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>23</v>
@@ -2551,16 +2557,16 @@
         <v>6</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D26" s="41">
         <v>30</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>23</v>
@@ -2579,10 +2585,10 @@
         <v>88</v>
       </c>
       <c r="D27" s="41"/>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="50"/>
+      <c r="F27" s="51"/>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
@@ -2600,7 +2606,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2622,7 +2628,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -2640,7 +2646,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -2660,7 +2666,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2712,7 +2718,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2762,7 +2768,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37" s="41">
         <v>5</v>
@@ -2785,7 +2791,7 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" s="41">
         <v>6</v>
@@ -2794,7 +2800,7 @@
         <v>131</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G38" t="s">
         <v>55</v>
@@ -2803,18 +2809,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" s="41">
         <v>7</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="F39" s="38" t="s">
         <v>129</v>
@@ -2831,16 +2837,16 @@
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D40" s="41">
         <v>8</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G40" t="s">
         <v>55</v>
@@ -2854,16 +2860,16 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D41" s="41">
         <v>9</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G41" t="s">
         <v>55</v>
@@ -2877,16 +2883,16 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D42" s="41">
         <v>10</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G42" t="s">
         <v>55</v>
@@ -2900,16 +2906,16 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D43" s="41">
         <v>11</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G43" t="s">
         <v>55</v>
@@ -2923,16 +2929,16 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G44" t="s">
         <v>55</v>
@@ -2946,39 +2952,31 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="51" t="s">
-        <v>156</v>
+        <v>166</v>
+      </c>
+      <c r="D45" s="43">
+        <v>12</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="F45" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="G45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+      <c r="F45" s="38"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>7</v>
       </c>
       <c r="C46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="D46" s="41" t="s">
+      <c r="F46" s="38" t="s">
         <v>158</v>
-      </c>
-      <c r="E46" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="F46" s="38" t="s">
-        <v>160</v>
       </c>
       <c r="G46" t="s">
         <v>55</v>
@@ -2987,21 +2985,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="G47" t="s">
         <v>55</v>
@@ -3011,7 +3009,27 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D48" s="41"/>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E48" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="F48" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="G48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D49" s="41"/>
@@ -3120,6 +3138,9 @@
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" s="41"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D85" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated Test cases and results (aft monday morning mtg)
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shu Yan\Desktop\Ulink\Documentation\Metrics\Bug Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP-GIT\Ulink\Documentation\Metrics\Bug Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="168">
   <si>
     <t>Task</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>Able to filter screenings for infant between 0 to 2 years old</t>
-  </si>
-  <si>
-    <t>13,14</t>
   </si>
   <si>
     <t>Screenings - sort</t>
@@ -557,6 +554,9 @@
   </si>
   <si>
     <t>Data not relevant or related message shown</t>
+  </si>
+  <si>
+    <t>Feature dropped</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -653,6 +653,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -871,6 +877,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1308,14 +1323,14 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
@@ -1341,7 +1356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1357,7 +1372,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="45">
         <v>2</v>
       </c>
@@ -1384,7 +1399,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
@@ -1409,7 +1424,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
@@ -1434,7 +1449,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
@@ -1450,7 +1465,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
@@ -1473,7 +1488,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
@@ -1496,7 +1511,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
@@ -1521,7 +1536,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
@@ -1545,7 +1560,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
         <v>27</v>
@@ -1563,7 +1578,7 @@
         <v>Fix during buffer time</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="49">
         <v>3</v>
       </c>
@@ -1589,7 +1604,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
@@ -1613,7 +1628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
@@ -1637,7 +1652,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="46" t="s">
         <v>42</v>
@@ -1652,7 +1667,7 @@
       </c>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
         <v>6</v>
       </c>
@@ -1676,7 +1691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="50"/>
       <c r="B17" s="50" t="s">
         <v>85</v>
@@ -1714,24 +1729,24 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="L22" sqref="L22:L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" customWidth="1"/>
-    <col min="3" max="3" width="36.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="38.54296875" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" customWidth="1"/>
-    <col min="12" max="12" width="34.81640625" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="35.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1769,7 +1784,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1845,7 +1860,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1875,7 +1890,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1892,7 +1907,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>51</v>
@@ -1901,13 +1916,13 @@
         <v>1</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1933,7 +1948,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J6" s="5">
         <v>42917</v>
@@ -1941,7 +1956,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1967,7 +1982,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J7" s="5">
         <v>42917</v>
@@ -1975,7 +1990,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2001,13 +2016,13 @@
         <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2033,13 +2048,13 @@
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2065,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J10" s="5">
         <v>42917</v>
@@ -2073,7 +2088,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -2090,7 +2105,7 @@
         <v>58</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>23</v>
@@ -2105,7 +2120,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2122,7 +2137,7 @@
         <v>65</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>23</v>
@@ -2135,7 +2150,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2161,13 +2176,13 @@
         <v>1</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2199,7 +2214,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>3</v>
@@ -2214,7 +2229,7 @@
         <v>58</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>23</v>
@@ -2229,7 +2244,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2237,16 +2252,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" s="41">
         <v>28</v>
       </c>
       <c r="E16" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="32" t="s">
         <v>123</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>124</v>
       </c>
       <c r="G16" s="23" t="s">
         <v>51</v>
@@ -2255,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J16" s="35">
         <v>42948</v>
@@ -2263,7 +2278,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2295,7 +2310,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -2327,7 +2342,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2359,7 +2374,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -2393,7 +2408,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -2401,7 +2416,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>112</v>
@@ -2425,99 +2440,93 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+    <row r="22" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52">
         <v>20</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="52">
         <v>6</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="40">
-        <v>12</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="D22" s="53"/>
+      <c r="E22" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="G22" s="7" t="s">
+      <c r="F22" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="7">
-        <v>1</v>
-      </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="5">
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="55">
         <v>42948</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+      <c r="K22" s="52"/>
+      <c r="L22" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="52">
         <v>21</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="52">
         <v>6</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="53"/>
+      <c r="E23" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="F23" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="7">
-        <v>5</v>
-      </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52">
         <v>22</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="52">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="D24" s="53"/>
+      <c r="E24" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="F24" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="7">
-        <v>5</v>
-      </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2525,16 +2534,16 @@
         <v>6</v>
       </c>
       <c r="C25" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="E25" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="F25" s="34" t="s">
         <v>118</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>119</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>51</v>
@@ -2549,7 +2558,7 @@
       <c r="K25" s="33"/>
       <c r="L25" s="33"/>
     </row>
-    <row r="26" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <v>24</v>
       </c>
@@ -2557,16 +2566,16 @@
         <v>6</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D26" s="41">
         <v>30</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>23</v>
@@ -2579,7 +2588,7 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="C27" s="30" t="s">
         <v>88</v>
@@ -2590,7 +2599,7 @@
       </c>
       <c r="F27" s="51"/>
     </row>
-    <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
@@ -2606,13 +2615,13 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -2628,13 +2637,13 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2646,13 +2655,13 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
@@ -2666,13 +2675,13 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2688,7 +2697,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2704,7 +2713,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -2718,13 +2727,13 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2740,21 +2749,21 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D36" s="41" t="s">
         <v>72</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G36" t="s">
         <v>51</v>
@@ -2763,44 +2772,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>7</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" s="41">
         <v>5</v>
       </c>
       <c r="E37" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="F37" s="38" t="s">
+      <c r="G37" t="s">
         <v>129</v>
-      </c>
-      <c r="G37" t="s">
-        <v>130</v>
       </c>
       <c r="H37">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D38" s="41">
         <v>6</v>
       </c>
       <c r="E38" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G38" t="s">
         <v>55</v>
@@ -2809,21 +2818,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D39" s="41">
         <v>7</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G39" t="s">
         <v>55</v>
@@ -2832,21 +2841,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D40" s="41">
         <v>8</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G40" t="s">
         <v>55</v>
@@ -2855,21 +2864,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D41" s="41">
         <v>9</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G41" t="s">
         <v>55</v>
@@ -2878,21 +2887,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D42" s="41">
         <v>10</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G42" t="s">
         <v>55</v>
@@ -2901,21 +2910,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D43" s="41">
         <v>11</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G43" t="s">
         <v>55</v>
@@ -2924,21 +2933,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G44" t="s">
         <v>55</v>
@@ -2947,36 +2956,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D45" s="43">
         <v>12</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F45" s="38"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D46" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E46" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="F46" s="38" t="s">
         <v>157</v>
-      </c>
-      <c r="F46" s="38" t="s">
-        <v>158</v>
       </c>
       <c r="G46" t="s">
         <v>55</v>
@@ -2985,21 +2994,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>7</v>
       </c>
       <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="E47" s="36" t="s">
+      <c r="F47" s="38" t="s">
         <v>155</v>
-      </c>
-      <c r="F47" s="38" t="s">
-        <v>156</v>
       </c>
       <c r="G47" t="s">
         <v>55</v>
@@ -3008,21 +3017,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E48" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48" s="38" t="s">
         <v>159</v>
-      </c>
-      <c r="F48" s="38" t="s">
-        <v>160</v>
       </c>
       <c r="G48" t="s">
         <v>55</v>
@@ -3031,115 +3040,115 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="41"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="41"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="41"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="41"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="41"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="41"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="41"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="41"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="41"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="41"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="41"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="41"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="41"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="41"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="41"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="41"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="41"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="41"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="41"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="41"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="41"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="41"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="41"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="41"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="41"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="41"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="41"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="41"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="41"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="41"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="41"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="41"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="41"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="41"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="41"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="41"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="41"/>
     </row>
   </sheetData>
@@ -3199,9 +3208,9 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="14" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L14">
         <v>0</v>
       </c>
@@ -3209,7 +3218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L15">
         <v>11</v>
       </c>
@@ -3217,7 +3226,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L16">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
update bug log for screenings
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP-GIT\Ulink\Documentation\Metrics\Bug Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shu Yan\Desktop\Ulink\Documentation\Metrics\Bug Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="1790" yWindow="470" windowWidth="25520" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
     <sheet name="Mitigation Plan" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
   <si>
     <t>Task</t>
   </si>
@@ -557,13 +557,91 @@
   </si>
   <si>
     <t>Feature dropped</t>
+  </si>
+  <si>
+    <t>in viewScreeningsAdult.html, upon clicking 'add new screening' , it should redirect to addscreeningadult.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direct to addscreening.html (for infant) </t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vaccination/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>screening</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vaccination / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Screening</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenings - Add (Infant) </t>
+  </si>
+  <si>
+    <t>Screenings - Add (Adults)</t>
+  </si>
+  <si>
+    <t>Screenings -  Link to Patient View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display male clients above 20 years olf for Cancers </t>
+  </si>
+  <si>
+    <t>Returned Client A, C,D,E,F whose gender are either male / female / blank</t>
+  </si>
+  <si>
+    <t>Should display infant for illness - pwqpqpw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Returned Client A, C,D,E,F, G whose age are above 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenings - sort adult </t>
+  </si>
+  <si>
+    <t>Gender = Male, the whole table shrink in size</t>
+  </si>
+  <si>
+    <t>After sorting gender = male, sort back to female and the table disappear, 'delete' was shown</t>
+  </si>
+  <si>
+    <t>After sorting gender = male, sort back to 'all', there is no change in result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenings - sort infant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">when sorting the age, illness and screening for infant, the data for infant changes to adult's </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +677,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -738,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -856,27 +948,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -886,6 +957,28 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1323,14 +1416,14 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
@@ -1356,7 +1449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1372,8 +1465,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="50">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1399,8 +1492,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="50"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1424,8 +1517,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="50"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1449,8 +1542,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="50"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -1465,8 +1558,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="50"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1488,8 +1581,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="50"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1511,8 +1604,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="50"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1536,8 +1629,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="50"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1560,15 +1653,15 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="46" t="s">
+    <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="50"/>
+      <c r="B11" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1578,8 +1671,8 @@
         <v>Fix during buffer time</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="49">
+    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="54">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1604,8 +1697,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="54"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1628,8 +1721,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="54"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
       </c>
@@ -1652,23 +1745,23 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="46" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="54"/>
+      <c r="B15" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
       </c>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="50">
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="55">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1691,15 +1784,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="55"/>
+      <c r="B17" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -1728,25 +1821,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22:L24"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.54296875" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="12" max="12" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1784,7 +1877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1822,7 +1915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1860,7 +1953,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1890,7 +1983,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1922,7 +2015,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1956,7 +2049,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1990,7 +2083,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2022,7 +2115,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2054,7 +2147,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2088,7 +2181,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -2120,7 +2213,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2150,7 +2243,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2182,7 +2275,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2214,7 +2307,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>3</v>
@@ -2244,7 +2337,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2278,7 +2371,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2310,7 +2403,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -2342,7 +2435,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2374,7 +2467,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -2408,7 +2501,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -2440,93 +2533,93 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+    <row r="22" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="45">
         <v>20</v>
       </c>
-      <c r="B22" s="52">
+      <c r="B22" s="45">
         <v>6</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="52" t="s">
+      <c r="D22" s="46"/>
+      <c r="E22" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="55">
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="48">
         <v>42948</v>
       </c>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52" t="s">
+      <c r="K22" s="45"/>
+      <c r="L22" s="45" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+    <row r="23" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="45">
         <v>21</v>
       </c>
-      <c r="B23" s="52">
+      <c r="B23" s="45">
         <v>6</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="52" t="s">
+      <c r="D23" s="46"/>
+      <c r="E23" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52" t="s">
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
+    <row r="24" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="45">
         <v>22</v>
       </c>
-      <c r="B24" s="52">
+      <c r="B24" s="45">
         <v>6</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="52" t="s">
+      <c r="D24" s="46"/>
+      <c r="E24" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="G24" s="52" t="s">
+      <c r="G24" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52" t="s">
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2558,7 +2651,7 @@
       <c r="K25" s="33"/>
       <c r="L25" s="33"/>
     </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="23">
         <v>24</v>
       </c>
@@ -2588,18 +2681,18 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
       <c r="C27" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="41"/>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="51"/>
-    </row>
-    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="F27" s="56"/>
+    </row>
+    <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
@@ -2621,7 +2714,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -2643,7 +2736,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2661,7 +2754,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
@@ -2681,7 +2774,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2697,7 +2790,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2713,7 +2806,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -2733,7 +2826,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2749,7 +2842,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>7</v>
       </c>
@@ -2772,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>7</v>
       </c>
@@ -2795,7 +2888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>7</v>
       </c>
@@ -2818,7 +2911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>7</v>
       </c>
@@ -2841,7 +2934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>7</v>
       </c>
@@ -2864,7 +2957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>7</v>
       </c>
@@ -2887,7 +2980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>7</v>
       </c>
@@ -2910,7 +3003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>7</v>
       </c>
@@ -2933,7 +3026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>7</v>
       </c>
@@ -2956,7 +3049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>7</v>
       </c>
@@ -2971,7 +3064,7 @@
       </c>
       <c r="F45" s="38"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>7</v>
       </c>
@@ -2994,7 +3087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>7</v>
       </c>
@@ -3017,7 +3110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>7</v>
       </c>
@@ -3040,115 +3133,221 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="41"/>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="G49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>173</v>
+      </c>
       <c r="D50" s="41"/>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="F50" s="57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>175</v>
+      </c>
       <c r="D51" s="41"/>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="G51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>175</v>
+      </c>
       <c r="D52" s="41"/>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="F52" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="G52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>180</v>
+      </c>
       <c r="D53" s="41"/>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="41"/>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F53" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="G53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="G54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>180</v>
+      </c>
       <c r="D55" s="41"/>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F55" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="G55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>184</v>
+      </c>
       <c r="D56" s="41"/>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="F56" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="G56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D57" s="41"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D58" s="41"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D59" s="41"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D60" s="41"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D61" s="41"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D62" s="41"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D63" s="41"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D64" s="41"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D65" s="41"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D66" s="41"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D67" s="41"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D68" s="41"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D69" s="41"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D70" s="41"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D71" s="41"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D72" s="41"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D73" s="41"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D74" s="41"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D75" s="41"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D76" s="41"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D77" s="41"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D78" s="41"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D79" s="41"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D80" s="41"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D81" s="41"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D82" s="41"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D83" s="41"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" s="41"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D85" s="41"/>
     </row>
   </sheetData>
@@ -3208,9 +3407,9 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="14" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L14">
         <v>0</v>
       </c>
@@ -3218,7 +3417,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L15">
         <v>11</v>
       </c>
@@ -3226,7 +3425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L16">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
update bug log for clients
see no changes in bootstrap function.
Clients
- drop down list not working
- appointment table shown for all clients even if theu have no
appointments
- screenings did not appear in each client info
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="196">
   <si>
     <t>Task</t>
   </si>
@@ -635,6 +635,36 @@
   </si>
   <si>
     <t xml:space="preserve">when sorting the age, illness and screening for infant, the data for infant changes to adult's </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client List - drop down list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no error / success message display, timestamp updated to current time, last three lines of the data file were also uploaded into database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table should show data based on the dropdown list </t>
+  </si>
+  <si>
+    <t>No change in table - data not sorted</t>
+  </si>
+  <si>
+    <t>View Client Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No screenings shown in each client info </t>
+  </si>
+  <si>
+    <t>Seach Box in Navigator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should show the various screenings for each client </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shouldn’t show in the header for all pages </t>
   </si>
 </sst>
 </file>
@@ -957,6 +987,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -978,7 +1009,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1466,7 +1496,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="50">
+      <c r="A3" s="51">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1493,7 +1523,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="50"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1518,7 +1548,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="50"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1543,7 +1573,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -1559,7 +1589,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1582,7 +1612,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1605,7 +1635,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1630,7 +1660,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1654,14 +1684,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1672,7 +1702,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="55">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1698,7 +1728,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="54"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1722,7 +1752,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="24" t="s">
         <v>47</v>
       </c>
@@ -1746,14 +1776,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
-      <c r="B15" s="51" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -1761,7 +1791,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="55">
+      <c r="A16" s="56">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1785,14 +1815,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="55" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -1819,10 +1849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2687,10 +2717,10 @@
         <v>88</v>
       </c>
       <c r="D27" s="41"/>
-      <c r="E27" s="56" t="s">
+      <c r="E27" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
@@ -3161,10 +3191,10 @@
         <v>173</v>
       </c>
       <c r="D50" s="41"/>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="F50" s="57" t="s">
+      <c r="F50" s="50" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3263,17 +3293,56 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>186</v>
+      </c>
       <c r="D57" s="41"/>
+      <c r="F57" s="38" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>187</v>
+      </c>
       <c r="D58" s="41"/>
+      <c r="E58" t="s">
+        <v>189</v>
+      </c>
+      <c r="F58" s="38" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>191</v>
+      </c>
       <c r="D59" s="41"/>
+      <c r="E59" t="s">
+        <v>194</v>
+      </c>
+      <c r="F59" s="38" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>193</v>
+      </c>
       <c r="D60" s="41"/>
+      <c r="E60" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D61" s="41"/>
@@ -3346,9 +3415,6 @@
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" s="41"/>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D85" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update bug log and result for iter 8 and 9 test cases
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="240">
   <si>
     <t>Task</t>
   </si>
@@ -683,6 +683,117 @@
   </si>
   <si>
     <t>unsolved</t>
+  </si>
+  <si>
+    <t>Requirements changed for bootstrap (extra column).Data file not suitable</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>864 Records loaded</t>
+  </si>
+  <si>
+    <t>0 Records loaded</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No response when clicking the generated result button. Should display result </t>
+  </si>
+  <si>
+    <t>Partial resolved. Medical working but not VISA</t>
+  </si>
+  <si>
+    <t>Report - KPI (VISA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report - KPI (Medical) </t>
+  </si>
+  <si>
+    <t>5,6,7,8</t>
+  </si>
+  <si>
+    <t>No figures for outpatient. Refer to test case for the expected result.</t>
+  </si>
+  <si>
+    <t>Have numbers for inpatient and outpatient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% calculation is wrong (0% for all) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month in "Compare with PREVIOUS YEAR" is wrong </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 to 10 </t>
+  </si>
+  <si>
+    <t>Rank Number is different as test case. Need to verify with KX / Linda</t>
+  </si>
+  <si>
+    <t>Name of referral / doctor/ screening are not in order. Need check with kx / linda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking - View Doctor List </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A total of 4 engagement by 2 doctors </t>
+  </si>
+  <si>
+    <t>multiple doctors shown, rank 1 has 9 engagement</t>
+  </si>
+  <si>
+    <t>Total 6 engegement by 4 doctors</t>
+  </si>
+  <si>
+    <t>5,7</t>
+  </si>
+  <si>
+    <t>Clinic missing</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than 1000 patients shown in graph (DB has 861 records / patients) </t>
+  </si>
+  <si>
+    <t>Dashboard - types of visa requested</t>
+  </si>
+  <si>
+    <t>Dashboard - VISA clients</t>
+  </si>
+  <si>
+    <t>Latest result is Dec, graph shows Jan - Jun</t>
+  </si>
+  <si>
+    <t>Dashboard - Medical Clients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard - top 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard - top 5 </t>
+  </si>
+  <si>
+    <t>Missing Graph</t>
+  </si>
+  <si>
+    <t>Gender Age Report</t>
+  </si>
+  <si>
+    <t>1 to 9</t>
+  </si>
+  <si>
+    <t>Jul, aug,sept,oct,nov,dec as latest data in db is dec</t>
+  </si>
+  <si>
+    <t>Female for all above 90% is wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a lot of doctor names are shown is wrong </t>
   </si>
 </sst>
 </file>
@@ -816,7 +927,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -887,11 +998,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1006,23 +1143,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1050,32 +1172,92 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -1544,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1600,7 +1782,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="45">
+      <c r="A3" s="59">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1627,7 +1809,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="45"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1652,7 +1834,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1677,7 +1859,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
@@ -1693,7 +1875,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1898,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1739,7 +1921,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="45"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
@@ -1764,7 +1946,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
@@ -1788,14 +1970,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
-      <c r="B11" s="46" t="s">
+      <c r="A11" s="59"/>
+      <c r="B11" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1806,7 +1988,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="49">
+      <c r="A12" s="63">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1832,7 +2014,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="49"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
       </c>
@@ -1856,7 +2038,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="49"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="24" t="s">
         <v>46</v>
       </c>
@@ -1880,14 +2062,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
-      <c r="B15" s="46" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -1895,7 +2077,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="50">
+      <c r="A16" s="64">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1919,22 +2101,85 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
       </c>
       <c r="H17" s="20"/>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="64">
+        <v>8</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" s="46">
+        <v>8</v>
+      </c>
+      <c r="D22" s="46">
+        <v>1</v>
+      </c>
+      <c r="E22" s="46">
+        <v>3</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="46">
+        <v>10</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="64"/>
+      <c r="B23" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="46">
+        <v>10</v>
+      </c>
+      <c r="D23" s="46">
+        <v>2</v>
+      </c>
+      <c r="E23" s="46">
+        <v>3</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="46">
+        <v>17</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="64"/>
+      <c r="B24" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="13">
+        <f>SUM(G22:G23)</f>
+        <v>27</v>
+      </c>
+      <c r="H24" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B24:F24"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B15:F15"/>
@@ -1943,7 +2188,7 @@
     <mergeCell ref="A16:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:F10">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1956,8 +2201,8 @@
   <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1966,7 +2211,7 @@
     <col min="2" max="2" width="5.81640625" customWidth="1"/>
     <col min="3" max="3" width="36.1796875" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="5" max="5" width="47" style="87" customWidth="1"/>
     <col min="6" max="6" width="38.54296875" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="10" max="10" width="12.81640625" customWidth="1"/>
@@ -1990,7 +2235,7 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="58" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2012,79 +2257,79 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52">
+    <row r="2" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="47">
         <v>1</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="47">
         <v>2</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="48">
         <v>2</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="52">
-        <v>5</v>
-      </c>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="47">
+        <v>5</v>
+      </c>
+      <c r="I2" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="J2" s="55">
+      <c r="J2" s="50">
         <v>42673</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="56" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52">
+    <row r="3" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="47">
         <v>2</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="47">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="53">
-        <v>5</v>
-      </c>
-      <c r="E3" s="52" t="s">
+      <c r="D3" s="48">
+        <v>5</v>
+      </c>
+      <c r="E3" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="52">
-        <v>5</v>
-      </c>
-      <c r="I3" s="57" t="s">
+      <c r="H3" s="47">
+        <v>5</v>
+      </c>
+      <c r="I3" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="50">
         <v>42673</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="47" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2101,7 +2346,7 @@
       <c r="D4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="80" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="27" t="s">
@@ -2133,7 +2378,7 @@
       <c r="D5" s="37">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="80" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="27" t="s">
@@ -2165,7 +2410,7 @@
       <c r="D6" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="80" t="s">
         <v>51</v>
       </c>
       <c r="F6" s="27" t="s">
@@ -2199,7 +2444,7 @@
       <c r="D7" s="37">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="80" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="27" t="s">
@@ -2233,7 +2478,7 @@
       <c r="D8" s="37">
         <v>13</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="80" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="27" t="s">
@@ -2265,7 +2510,7 @@
       <c r="D9" s="37">
         <v>14</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="80" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="27" t="s">
@@ -2297,7 +2542,7 @@
       <c r="D10" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="80" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="27" t="s">
@@ -2331,7 +2576,7 @@
       <c r="D11" s="37">
         <v>18</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="80" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="27" t="s">
@@ -2363,7 +2608,7 @@
       <c r="D12" s="37">
         <v>19</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="80" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="27" t="s">
@@ -2393,7 +2638,7 @@
       <c r="D13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="80" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="27" t="s">
@@ -2425,7 +2670,7 @@
       <c r="D14" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="80" t="s">
         <v>61</v>
       </c>
       <c r="F14" s="27" t="s">
@@ -2455,7 +2700,7 @@
       <c r="D15" s="38">
         <v>27</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="80" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="31" t="s">
@@ -2487,7 +2732,7 @@
       <c r="D16" s="38">
         <v>28</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="81" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="31" t="s">
@@ -2521,7 +2766,7 @@
       <c r="D17" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="82" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="28" t="s">
@@ -2553,7 +2798,7 @@
       <c r="D18" s="37">
         <v>7</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="82" t="s">
         <v>108</v>
       </c>
       <c r="F18" s="28" t="s">
@@ -2585,7 +2830,7 @@
       <c r="D19" s="37">
         <v>6</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="82" t="s">
         <v>76</v>
       </c>
       <c r="F19" s="28" t="s">
@@ -2617,7 +2862,7 @@
       <c r="D20" s="37">
         <v>8</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="82" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="28" t="s">
@@ -2651,7 +2896,7 @@
       <c r="D21" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="82" t="s">
         <v>81</v>
       </c>
       <c r="F21" s="28" t="s">
@@ -2681,7 +2926,7 @@
         <v>82</v>
       </c>
       <c r="D22" s="41"/>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="83" t="s">
         <v>113</v>
       </c>
       <c r="F22" s="42" t="s">
@@ -2711,7 +2956,7 @@
         <v>82</v>
       </c>
       <c r="D23" s="41"/>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="83" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="42" t="s">
@@ -2739,7 +2984,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="41"/>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="83" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="42" t="s">
@@ -2769,7 +3014,7 @@
       <c r="D25" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="81" t="s">
         <v>116</v>
       </c>
       <c r="F25" s="33" t="s">
@@ -2803,7 +3048,7 @@
       <c r="D26" s="38">
         <v>30</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="81" t="s">
         <v>136</v>
       </c>
       <c r="F26" s="35" t="s">
@@ -2828,10 +3073,10 @@
         <v>87</v>
       </c>
       <c r="D27" s="38"/>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="51"/>
+      <c r="F27" s="65"/>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
@@ -2842,7 +3087,7 @@
         <v>86</v>
       </c>
       <c r="D28" s="37"/>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="80" t="s">
         <v>88</v>
       </c>
       <c r="F28" s="28" t="s">
@@ -2866,7 +3111,7 @@
         <v>86</v>
       </c>
       <c r="D29" s="37"/>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="80" t="s">
         <v>89</v>
       </c>
       <c r="F29" s="28" t="s">
@@ -2888,7 +3133,7 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="37"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="80"/>
       <c r="F30" s="28" t="s">
         <v>101</v>
       </c>
@@ -2910,7 +3155,7 @@
         <v>70</v>
       </c>
       <c r="D31" s="37"/>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="80" t="s">
         <v>93</v>
       </c>
       <c r="F31" s="4"/>
@@ -2930,7 +3175,7 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="37"/>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="80" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="4"/>
@@ -2952,7 +3197,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="37"/>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="80" t="s">
         <v>95</v>
       </c>
       <c r="F33" s="4"/>
@@ -2974,7 +3219,7 @@
         <v>96</v>
       </c>
       <c r="D34" s="37"/>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="80" t="s">
         <v>97</v>
       </c>
       <c r="F34" s="4"/>
@@ -2994,7 +3239,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="37"/>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="53" t="s">
         <v>98</v>
       </c>
       <c r="F35" s="4"/>
@@ -3020,10 +3265,10 @@
       <c r="D36" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="F36" s="59" t="s">
+      <c r="F36" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -3032,10 +3277,14 @@
       <c r="H36" s="4">
         <v>1</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="L36" s="66" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
@@ -3050,10 +3299,10 @@
       <c r="D37" s="37">
         <v>5</v>
       </c>
-      <c r="E37" s="58" t="s">
+      <c r="E37" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="F37" s="59" t="s">
+      <c r="F37" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -3062,10 +3311,12 @@
       <c r="H37" s="4">
         <v>5</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
+      <c r="L37" s="67"/>
     </row>
     <row r="38" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
@@ -3080,10 +3331,10 @@
       <c r="D38" s="37">
         <v>6</v>
       </c>
-      <c r="E38" s="58" t="s">
+      <c r="E38" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="F38" s="59" t="s">
+      <c r="F38" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -3092,10 +3343,12 @@
       <c r="H38" s="4">
         <v>5</v>
       </c>
-      <c r="I38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
+      <c r="L38" s="67"/>
     </row>
     <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
@@ -3110,10 +3363,10 @@
       <c r="D39" s="37">
         <v>7</v>
       </c>
-      <c r="E39" s="58" t="s">
+      <c r="E39" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="F39" s="59" t="s">
+      <c r="F39" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -3122,10 +3375,12 @@
       <c r="H39" s="4">
         <v>5</v>
       </c>
-      <c r="I39" s="4"/>
+      <c r="I39" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
+      <c r="L39" s="67"/>
     </row>
     <row r="40" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
@@ -3140,10 +3395,10 @@
       <c r="D40" s="37">
         <v>8</v>
       </c>
-      <c r="E40" s="58" t="s">
+      <c r="E40" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="F40" s="59" t="s">
+      <c r="F40" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -3152,10 +3407,12 @@
       <c r="H40" s="4">
         <v>5</v>
       </c>
-      <c r="I40" s="4"/>
+      <c r="I40" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
+      <c r="L40" s="67"/>
     </row>
     <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
@@ -3170,10 +3427,10 @@
       <c r="D41" s="37">
         <v>9</v>
       </c>
-      <c r="E41" s="58" t="s">
+      <c r="E41" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="F41" s="59" t="s">
+      <c r="F41" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -3182,10 +3439,12 @@
       <c r="H41" s="4">
         <v>5</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="I41" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
+      <c r="L41" s="67"/>
     </row>
     <row r="42" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
@@ -3200,10 +3459,10 @@
       <c r="D42" s="37">
         <v>10</v>
       </c>
-      <c r="E42" s="58" t="s">
+      <c r="E42" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="F42" s="59" t="s">
+      <c r="F42" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -3212,10 +3471,12 @@
       <c r="H42" s="4">
         <v>5</v>
       </c>
-      <c r="I42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
+      <c r="L42" s="67"/>
     </row>
     <row r="43" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
@@ -3230,10 +3491,10 @@
       <c r="D43" s="37">
         <v>11</v>
       </c>
-      <c r="E43" s="58" t="s">
+      <c r="E43" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="F43" s="59" t="s">
+      <c r="F43" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -3242,10 +3503,12 @@
       <c r="H43" s="4">
         <v>5</v>
       </c>
-      <c r="I43" s="4"/>
+      <c r="I43" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
+      <c r="L43" s="67"/>
     </row>
     <row r="44" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
@@ -3257,13 +3520,13 @@
       <c r="C44" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="60" t="s">
+      <c r="D44" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="E44" s="58" t="s">
+      <c r="E44" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="59" t="s">
+      <c r="F44" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -3272,10 +3535,12 @@
       <c r="H44" s="4">
         <v>5</v>
       </c>
-      <c r="I44" s="4"/>
+      <c r="I44" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
+      <c r="L44" s="67"/>
     </row>
     <row r="45" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
@@ -3287,23 +3552,25 @@
       <c r="C45" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D45" s="60">
+      <c r="D45" s="55">
         <v>12</v>
       </c>
-      <c r="E45" s="58" t="s">
+      <c r="E45" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="F45" s="59" t="s">
+      <c r="F45" s="54" t="s">
         <v>194</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
+      <c r="I45" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J45" s="4"/>
       <c r="K45" s="5">
         <v>42757</v>
       </c>
-      <c r="L45" s="4"/>
+      <c r="L45" s="68"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
@@ -3315,13 +3582,13 @@
       <c r="C46" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="61" t="s">
+      <c r="D46" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="E46" s="58" t="s">
+      <c r="E46" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="F46" s="59" t="s">
+      <c r="F46" s="54" t="s">
         <v>148</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -3350,10 +3617,10 @@
       <c r="D47" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="E47" s="58" t="s">
+      <c r="E47" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="F47" s="59" t="s">
+      <c r="F47" s="54" t="s">
         <v>146</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -3384,10 +3651,10 @@
       <c r="D48" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="E48" s="58" t="s">
+      <c r="E48" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="F48" s="59" t="s">
+      <c r="F48" s="54" t="s">
         <v>150</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -3418,10 +3685,10 @@
       <c r="D49" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="58" t="s">
+      <c r="E49" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="F49" s="59" t="s">
+      <c r="F49" s="54" t="s">
         <v>160</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -3448,10 +3715,10 @@
         <v>164</v>
       </c>
       <c r="D50" s="37"/>
-      <c r="E50" s="62" t="s">
+      <c r="E50" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="57" t="s">
         <v>162</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -3476,10 +3743,10 @@
         <v>166</v>
       </c>
       <c r="D51" s="37"/>
-      <c r="E51" s="58" t="s">
+      <c r="E51" s="53" t="s">
         <v>189</v>
       </c>
-      <c r="F51" s="59" t="s">
+      <c r="F51" s="54" t="s">
         <v>167</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -3504,10 +3771,10 @@
         <v>166</v>
       </c>
       <c r="D52" s="37"/>
-      <c r="E52" s="58" t="s">
+      <c r="E52" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="F52" s="59" t="s">
+      <c r="F52" s="54" t="s">
         <v>169</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -3532,8 +3799,8 @@
         <v>170</v>
       </c>
       <c r="D53" s="37"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="59" t="s">
+      <c r="E53" s="80"/>
+      <c r="F53" s="54" t="s">
         <v>171</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -3562,8 +3829,8 @@
         <v>170</v>
       </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="59" t="s">
+      <c r="E54" s="80"/>
+      <c r="F54" s="54" t="s">
         <v>173</v>
       </c>
       <c r="G54" s="4" t="s">
@@ -3592,8 +3859,8 @@
         <v>170</v>
       </c>
       <c r="D55" s="37"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="59" t="s">
+      <c r="E55" s="80"/>
+      <c r="F55" s="54" t="s">
         <v>172</v>
       </c>
       <c r="G55" s="4" t="s">
@@ -3622,8 +3889,8 @@
         <v>174</v>
       </c>
       <c r="D56" s="37"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="59" t="s">
+      <c r="E56" s="80"/>
+      <c r="F56" s="54" t="s">
         <v>175</v>
       </c>
       <c r="G56" s="4" t="s">
@@ -3652,8 +3919,8 @@
         <v>193</v>
       </c>
       <c r="D57" s="37"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="59" t="s">
+      <c r="E57" s="80"/>
+      <c r="F57" s="54" t="s">
         <v>195</v>
       </c>
       <c r="G57" s="4" t="s">
@@ -3678,10 +3945,10 @@
         <v>176</v>
       </c>
       <c r="D58" s="37"/>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="F58" s="59" t="s">
+      <c r="F58" s="54" t="s">
         <v>178</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -3710,10 +3977,10 @@
         <v>179</v>
       </c>
       <c r="D59" s="37"/>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="F59" s="59" t="s">
+      <c r="F59" s="54" t="s">
         <v>180</v>
       </c>
       <c r="G59" s="4" t="s">
@@ -3739,8 +4006,8 @@
       <c r="C60" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D60" s="60"/>
-      <c r="E60" s="4" t="s">
+      <c r="D60" s="55"/>
+      <c r="E60" s="80" t="s">
         <v>183</v>
       </c>
       <c r="F60" s="4"/>
@@ -3769,8 +4036,8 @@
       <c r="C61" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D61" s="60"/>
-      <c r="E61" s="4" t="s">
+      <c r="D61" s="55"/>
+      <c r="E61" s="80" t="s">
         <v>191</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -3799,8 +4066,8 @@
       <c r="C62" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D62" s="60"/>
-      <c r="E62" s="27" t="s">
+      <c r="D62" s="55"/>
+      <c r="E62" s="53" t="s">
         <v>192</v>
       </c>
       <c r="F62" s="4"/>
@@ -3827,11 +4094,11 @@
       <c r="C63" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D63" s="60"/>
-      <c r="E63" s="27" t="s">
+      <c r="D63" s="55"/>
+      <c r="E63" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="78" t="s">
         <v>200</v>
       </c>
       <c r="G63" s="4" t="s">
@@ -3849,7 +4116,7 @@
     </row>
     <row r="64" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B64" s="4">
         <v>7</v>
@@ -3857,8 +4124,8 @@
       <c r="C64" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D64" s="60"/>
-      <c r="E64" s="27" t="s">
+      <c r="D64" s="55"/>
+      <c r="E64" s="53" t="s">
         <v>199</v>
       </c>
       <c r="F64" s="4"/>
@@ -3876,122 +4143,562 @@
       <c r="L64" s="4"/>
     </row>
     <row r="65" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="4">
-        <v>60</v>
-      </c>
-      <c r="B65" s="4">
+      <c r="A65" s="70">
+        <v>62</v>
+      </c>
+      <c r="B65" s="70">
         <v>8</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="70" t="s">
         <v>184</v>
       </c>
-      <c r="D65" s="37"/>
-      <c r="E65" s="27" t="s">
+      <c r="D65" s="69"/>
+      <c r="E65" s="85" t="s">
         <v>185</v>
       </c>
-      <c r="F65" s="59" t="s">
+      <c r="F65" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="H65" s="4">
-        <v>5</v>
-      </c>
-      <c r="I65" s="30"/>
-      <c r="J65" s="5">
+      <c r="H65" s="70">
+        <v>5</v>
+      </c>
+      <c r="I65" s="73"/>
+      <c r="J65" s="74">
         <v>42757</v>
       </c>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
+      <c r="K65" s="70"/>
+      <c r="L65" s="71" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D66" s="38"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D67" s="38"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D68" s="38"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D69" s="38"/>
+      <c r="A66" s="4">
+        <v>63</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D66" s="37"/>
+      <c r="E66" s="80" t="s">
+        <v>205</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H66" s="7">
+        <v>5</v>
+      </c>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="4">
+        <v>64</v>
+      </c>
+      <c r="B67" s="4">
+        <v>8</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D67" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E67" s="80"/>
+      <c r="F67" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="4">
+        <v>5</v>
+      </c>
+      <c r="I67" s="4"/>
+      <c r="J67" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+    </row>
+    <row r="68" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="4">
+        <v>65</v>
+      </c>
+      <c r="B68" s="4">
+        <v>8</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="E68" s="86" t="s">
+        <v>214</v>
+      </c>
+      <c r="F68" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="4">
+        <v>5</v>
+      </c>
+      <c r="I68" s="4"/>
+      <c r="J68" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+    </row>
+    <row r="69" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="4">
+        <v>66</v>
+      </c>
+      <c r="B69" s="4">
+        <v>8</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="E69" s="86"/>
+      <c r="F69" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H69" s="4">
+        <v>1</v>
+      </c>
+      <c r="I69" s="4"/>
+      <c r="J69" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D70" s="38"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D71" s="38"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D72" s="38"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D73" s="38"/>
+      <c r="A70" s="4">
+        <v>67</v>
+      </c>
+      <c r="B70" s="4">
+        <v>8</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="E70" s="80"/>
+      <c r="F70" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="4">
+        <v>5</v>
+      </c>
+      <c r="I70" s="4"/>
+      <c r="J70" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+    </row>
+    <row r="71" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="4">
+        <v>68</v>
+      </c>
+      <c r="B71" s="4">
+        <v>8</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="E71" s="80"/>
+      <c r="F71" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="4">
+        <v>1</v>
+      </c>
+      <c r="I71" s="4"/>
+      <c r="J71" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="4">
+        <v>69</v>
+      </c>
+      <c r="B72" s="4">
+        <v>8</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="E72" s="80"/>
+      <c r="F72" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H72" s="4">
+        <v>1</v>
+      </c>
+      <c r="I72" s="4"/>
+      <c r="J72" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+    </row>
+    <row r="73" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="4">
+        <v>70</v>
+      </c>
+      <c r="B73" s="4">
+        <v>8</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D73" s="37">
+        <v>5</v>
+      </c>
+      <c r="E73" s="80" t="s">
+        <v>221</v>
+      </c>
+      <c r="F73" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H73" s="4">
+        <v>5</v>
+      </c>
+      <c r="I73" s="4"/>
+      <c r="J73" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D74" s="38"/>
+      <c r="A74" s="4">
+        <v>71</v>
+      </c>
+      <c r="B74" s="4">
+        <v>8</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" s="37">
+        <v>7</v>
+      </c>
+      <c r="E74" s="80" t="s">
+        <v>223</v>
+      </c>
+      <c r="F74" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H74" s="7">
+        <v>5</v>
+      </c>
+      <c r="I74" s="4"/>
+      <c r="J74" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D75" s="38"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D76" s="38"/>
+      <c r="A75" s="4">
+        <v>72</v>
+      </c>
+      <c r="B75" s="4">
+        <v>8</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D75" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="E75" s="80"/>
+      <c r="F75" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H75" s="4">
+        <v>5</v>
+      </c>
+      <c r="I75" s="4"/>
+      <c r="J75" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+    </row>
+    <row r="76" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="4">
+        <v>73</v>
+      </c>
+      <c r="B76" s="7">
+        <v>9</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D76" s="37">
+        <v>1</v>
+      </c>
+      <c r="E76" s="80"/>
+      <c r="F76" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H76" s="4">
+        <v>5</v>
+      </c>
+      <c r="I76" s="4"/>
+      <c r="J76" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D77" s="38"/>
+      <c r="A77" s="4">
+        <v>74</v>
+      </c>
+      <c r="B77" s="7">
+        <v>9</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D77" s="37">
+        <v>2</v>
+      </c>
+      <c r="E77" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F77" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" s="4">
+        <v>5</v>
+      </c>
+      <c r="I77" s="4"/>
+      <c r="J77" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D78" s="38"/>
+      <c r="A78" s="4">
+        <v>75</v>
+      </c>
+      <c r="B78" s="7">
+        <v>9</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D78" s="37">
+        <v>3</v>
+      </c>
+      <c r="E78" s="77"/>
+      <c r="F78" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H78" s="4">
+        <v>5</v>
+      </c>
+      <c r="I78" s="4"/>
+      <c r="J78" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D79" s="38"/>
+      <c r="A79" s="4">
+        <v>76</v>
+      </c>
+      <c r="B79" s="7">
+        <v>9</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D79" s="37">
+        <v>4</v>
+      </c>
+      <c r="E79" s="80"/>
+      <c r="F79" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H79" s="4">
+        <v>5</v>
+      </c>
+      <c r="I79" s="4"/>
+      <c r="J79" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D80" s="38"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D81" s="38"/>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="4">
+        <v>77</v>
+      </c>
+      <c r="B80" s="7">
+        <v>9</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D80" s="37">
+        <v>5</v>
+      </c>
+      <c r="E80" s="80"/>
+      <c r="F80" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80" s="4">
+        <v>5</v>
+      </c>
+      <c r="I80" s="4"/>
+      <c r="J80" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A81" s="4">
+        <v>78</v>
+      </c>
+      <c r="B81" s="7">
+        <v>9</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="E81" s="80"/>
+      <c r="F81" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H81" s="7">
+        <v>5</v>
+      </c>
+      <c r="I81" s="4"/>
+      <c r="J81" s="5">
+        <v>42772</v>
+      </c>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D82" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="E27:F27"/>
+    <mergeCell ref="L36:L45"/>
+    <mergeCell ref="E77:E78"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:I13">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"unsolve"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update testcases and metrics
ranking function - rank (number) and order affected
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="236">
   <si>
     <t>Task</t>
   </si>
@@ -727,15 +727,6 @@
     <t xml:space="preserve">Month in "Compare with PREVIOUS YEAR" is wrong </t>
   </si>
   <si>
-    <t xml:space="preserve">1 to 10 </t>
-  </si>
-  <si>
-    <t>Rank Number is different as test case. Need to verify with KX / Linda</t>
-  </si>
-  <si>
-    <t>Name of referral / doctor/ screening are not in order. Need check with kx / linda</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ranking - View Doctor List </t>
   </si>
   <si>
@@ -748,12 +739,6 @@
     <t>Total 6 engegement by 4 doctors</t>
   </si>
   <si>
-    <t>5,7</t>
-  </si>
-  <si>
-    <t>Clinic missing</t>
-  </si>
-  <si>
     <t>Report</t>
   </si>
   <si>
@@ -794,6 +779,9 @@
   </si>
   <si>
     <t xml:space="preserve">a lot of doctor names are shown is wrong </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1172,35 +1160,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1217,40 +1178,70 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1729,7 +1720,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1782,7 +1773,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="59">
+      <c r="A3" s="78">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1809,7 +1800,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="59"/>
+      <c r="A4" s="78"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1834,7 +1825,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="59"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1859,7 +1850,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
@@ -1875,7 +1866,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="59"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1898,7 +1889,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="59"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1921,7 +1912,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
@@ -1946,7 +1937,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
@@ -1970,14 +1961,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="81"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1988,7 +1979,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="63">
+      <c r="A12" s="82">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -2014,7 +2005,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="63"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
       </c>
@@ -2038,7 +2029,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="63"/>
+      <c r="A14" s="82"/>
       <c r="B14" s="24" t="s">
         <v>46</v>
       </c>
@@ -2062,14 +2053,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="63"/>
-      <c r="B15" s="60" t="s">
+      <c r="A15" s="82"/>
+      <c r="B15" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="62"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="81"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -2077,7 +2068,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="64">
+      <c r="A16" s="77">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -2101,26 +2092,26 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64" t="s">
+      <c r="A17" s="77"/>
+      <c r="B17" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
       </c>
       <c r="H17" s="20"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="64">
+    <row r="22" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="77">
         <v>8</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C22" s="46">
         <v>8</v>
@@ -2133,46 +2124,46 @@
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="46">
-        <v>10</v>
-      </c>
-      <c r="H22" s="46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="64"/>
+        <v>16</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="77"/>
       <c r="B23" s="26" t="s">
         <v>207</v>
       </c>
       <c r="C23" s="46">
         <v>10</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="E23" s="46">
         <v>2</v>
-      </c>
-      <c r="E23" s="46">
-        <v>3</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="46">
-        <v>17</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>68</v>
+        <v>10</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64" t="s">
+      <c r="A24" s="77"/>
+      <c r="B24" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
       <c r="G24" s="13">
         <f>SUM(G22:G23)</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H24" s="45"/>
     </row>
@@ -2198,11 +2189,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2211,7 +2202,7 @@
     <col min="2" max="2" width="5.81640625" customWidth="1"/>
     <col min="3" max="3" width="36.1796875" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47" style="87" customWidth="1"/>
+    <col min="5" max="5" width="47" style="76" customWidth="1"/>
     <col min="6" max="6" width="38.54296875" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="10" max="10" width="12.81640625" customWidth="1"/>
@@ -2270,7 +2261,7 @@
       <c r="D2" s="48">
         <v>2</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="68" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="49" t="s">
@@ -2308,7 +2299,7 @@
       <c r="D3" s="48">
         <v>5</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="68" t="s">
         <v>38</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -2346,7 +2337,7 @@
       <c r="D4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="69" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="27" t="s">
@@ -2378,7 +2369,7 @@
       <c r="D5" s="37">
         <v>7</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="69" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="27" t="s">
@@ -2410,7 +2401,7 @@
       <c r="D6" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="69" t="s">
         <v>51</v>
       </c>
       <c r="F6" s="27" t="s">
@@ -2444,7 +2435,7 @@
       <c r="D7" s="37">
         <v>12</v>
       </c>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="69" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="27" t="s">
@@ -2478,7 +2469,7 @@
       <c r="D8" s="37">
         <v>13</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="69" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="27" t="s">
@@ -2510,7 +2501,7 @@
       <c r="D9" s="37">
         <v>14</v>
       </c>
-      <c r="E9" s="80" t="s">
+      <c r="E9" s="69" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="27" t="s">
@@ -2542,7 +2533,7 @@
       <c r="D10" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="80" t="s">
+      <c r="E10" s="69" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="27" t="s">
@@ -2576,7 +2567,7 @@
       <c r="D11" s="37">
         <v>18</v>
       </c>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="69" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="27" t="s">
@@ -2608,7 +2599,7 @@
       <c r="D12" s="37">
         <v>19</v>
       </c>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="69" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="27" t="s">
@@ -2638,7 +2629,7 @@
       <c r="D13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="69" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="27" t="s">
@@ -2670,7 +2661,7 @@
       <c r="D14" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="80" t="s">
+      <c r="E14" s="69" t="s">
         <v>61</v>
       </c>
       <c r="F14" s="27" t="s">
@@ -2700,7 +2691,7 @@
       <c r="D15" s="38">
         <v>27</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="69" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="31" t="s">
@@ -2732,7 +2723,7 @@
       <c r="D16" s="38">
         <v>28</v>
       </c>
-      <c r="E16" s="81" t="s">
+      <c r="E16" s="70" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="31" t="s">
@@ -2766,7 +2757,7 @@
       <c r="D17" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="82" t="s">
+      <c r="E17" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="28" t="s">
@@ -2798,7 +2789,7 @@
       <c r="D18" s="37">
         <v>7</v>
       </c>
-      <c r="E18" s="82" t="s">
+      <c r="E18" s="71" t="s">
         <v>108</v>
       </c>
       <c r="F18" s="28" t="s">
@@ -2830,7 +2821,7 @@
       <c r="D19" s="37">
         <v>6</v>
       </c>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="71" t="s">
         <v>76</v>
       </c>
       <c r="F19" s="28" t="s">
@@ -2862,7 +2853,7 @@
       <c r="D20" s="37">
         <v>8</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="71" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="28" t="s">
@@ -2896,7 +2887,7 @@
       <c r="D21" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="71" t="s">
         <v>81</v>
       </c>
       <c r="F21" s="28" t="s">
@@ -2926,7 +2917,7 @@
         <v>82</v>
       </c>
       <c r="D22" s="41"/>
-      <c r="E22" s="83" t="s">
+      <c r="E22" s="72" t="s">
         <v>113</v>
       </c>
       <c r="F22" s="42" t="s">
@@ -2956,7 +2947,7 @@
         <v>82</v>
       </c>
       <c r="D23" s="41"/>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="72" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="42" t="s">
@@ -2984,7 +2975,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="41"/>
-      <c r="E24" s="83" t="s">
+      <c r="E24" s="72" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="42" t="s">
@@ -3014,7 +3005,7 @@
       <c r="D25" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="81" t="s">
+      <c r="E25" s="70" t="s">
         <v>116</v>
       </c>
       <c r="F25" s="33" t="s">
@@ -3048,7 +3039,7 @@
       <c r="D26" s="38">
         <v>30</v>
       </c>
-      <c r="E26" s="81" t="s">
+      <c r="E26" s="70" t="s">
         <v>136</v>
       </c>
       <c r="F26" s="35" t="s">
@@ -3073,10 +3064,10 @@
         <v>87</v>
       </c>
       <c r="D27" s="38"/>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="65"/>
+      <c r="F27" s="83"/>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
@@ -3087,7 +3078,7 @@
         <v>86</v>
       </c>
       <c r="D28" s="37"/>
-      <c r="E28" s="80" t="s">
+      <c r="E28" s="69" t="s">
         <v>88</v>
       </c>
       <c r="F28" s="28" t="s">
@@ -3111,7 +3102,7 @@
         <v>86</v>
       </c>
       <c r="D29" s="37"/>
-      <c r="E29" s="80" t="s">
+      <c r="E29" s="69" t="s">
         <v>89</v>
       </c>
       <c r="F29" s="28" t="s">
@@ -3133,7 +3124,7 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="37"/>
-      <c r="E30" s="80"/>
+      <c r="E30" s="69"/>
       <c r="F30" s="28" t="s">
         <v>101</v>
       </c>
@@ -3155,7 +3146,7 @@
         <v>70</v>
       </c>
       <c r="D31" s="37"/>
-      <c r="E31" s="80" t="s">
+      <c r="E31" s="69" t="s">
         <v>93</v>
       </c>
       <c r="F31" s="4"/>
@@ -3175,7 +3166,7 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="37"/>
-      <c r="E32" s="80" t="s">
+      <c r="E32" s="69" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="4"/>
@@ -3197,7 +3188,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="37"/>
-      <c r="E33" s="80" t="s">
+      <c r="E33" s="69" t="s">
         <v>95</v>
       </c>
       <c r="F33" s="4"/>
@@ -3219,7 +3210,7 @@
         <v>96</v>
       </c>
       <c r="D34" s="37"/>
-      <c r="E34" s="80" t="s">
+      <c r="E34" s="69" t="s">
         <v>97</v>
       </c>
       <c r="F34" s="4"/>
@@ -3282,7 +3273,7 @@
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="66" t="s">
+      <c r="L36" s="84" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3316,7 +3307,7 @@
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="67"/>
+      <c r="L37" s="85"/>
     </row>
     <row r="38" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
@@ -3348,7 +3339,7 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="67"/>
+      <c r="L38" s="85"/>
     </row>
     <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
@@ -3380,7 +3371,7 @@
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="67"/>
+      <c r="L39" s="85"/>
     </row>
     <row r="40" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
@@ -3412,7 +3403,7 @@
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="67"/>
+      <c r="L40" s="85"/>
     </row>
     <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
@@ -3444,7 +3435,7 @@
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="67"/>
+      <c r="L41" s="85"/>
     </row>
     <row r="42" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
@@ -3476,7 +3467,7 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="67"/>
+      <c r="L42" s="85"/>
     </row>
     <row r="43" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
@@ -3508,7 +3499,7 @@
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="67"/>
+      <c r="L43" s="85"/>
     </row>
     <row r="44" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
@@ -3540,7 +3531,7 @@
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="67"/>
+      <c r="L44" s="85"/>
     </row>
     <row r="45" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
@@ -3570,7 +3561,7 @@
       <c r="K45" s="5">
         <v>42757</v>
       </c>
-      <c r="L45" s="68"/>
+      <c r="L45" s="86"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
@@ -3715,7 +3706,7 @@
         <v>164</v>
       </c>
       <c r="D50" s="37"/>
-      <c r="E50" s="84" t="s">
+      <c r="E50" s="73" t="s">
         <v>163</v>
       </c>
       <c r="F50" s="57" t="s">
@@ -3799,7 +3790,7 @@
         <v>170</v>
       </c>
       <c r="D53" s="37"/>
-      <c r="E53" s="80"/>
+      <c r="E53" s="69"/>
       <c r="F53" s="54" t="s">
         <v>171</v>
       </c>
@@ -3829,7 +3820,7 @@
         <v>170</v>
       </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="80"/>
+      <c r="E54" s="69"/>
       <c r="F54" s="54" t="s">
         <v>173</v>
       </c>
@@ -3859,7 +3850,7 @@
         <v>170</v>
       </c>
       <c r="D55" s="37"/>
-      <c r="E55" s="80"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="54" t="s">
         <v>172</v>
       </c>
@@ -3889,7 +3880,7 @@
         <v>174</v>
       </c>
       <c r="D56" s="37"/>
-      <c r="E56" s="80"/>
+      <c r="E56" s="69"/>
       <c r="F56" s="54" t="s">
         <v>175</v>
       </c>
@@ -3919,7 +3910,7 @@
         <v>193</v>
       </c>
       <c r="D57" s="37"/>
-      <c r="E57" s="80"/>
+      <c r="E57" s="69"/>
       <c r="F57" s="54" t="s">
         <v>195</v>
       </c>
@@ -3945,7 +3936,7 @@
         <v>176</v>
       </c>
       <c r="D58" s="37"/>
-      <c r="E58" s="80" t="s">
+      <c r="E58" s="69" t="s">
         <v>177</v>
       </c>
       <c r="F58" s="54" t="s">
@@ -3977,7 +3968,7 @@
         <v>179</v>
       </c>
       <c r="D59" s="37"/>
-      <c r="E59" s="80" t="s">
+      <c r="E59" s="69" t="s">
         <v>182</v>
       </c>
       <c r="F59" s="54" t="s">
@@ -4007,7 +3998,7 @@
         <v>181</v>
       </c>
       <c r="D60" s="55"/>
-      <c r="E60" s="80" t="s">
+      <c r="E60" s="69" t="s">
         <v>183</v>
       </c>
       <c r="F60" s="4"/>
@@ -4037,7 +4028,7 @@
         <v>170</v>
       </c>
       <c r="D61" s="55"/>
-      <c r="E61" s="80" t="s">
+      <c r="E61" s="69" t="s">
         <v>191</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -4098,7 +4089,7 @@
       <c r="E63" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="F63" s="78" t="s">
+      <c r="F63" s="67" t="s">
         <v>200</v>
       </c>
       <c r="G63" s="4" t="s">
@@ -4143,34 +4134,34 @@
       <c r="L64" s="4"/>
     </row>
     <row r="65" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="70">
+      <c r="A65" s="61">
         <v>62</v>
       </c>
-      <c r="B65" s="70">
+      <c r="B65" s="61">
         <v>8</v>
       </c>
-      <c r="C65" s="70" t="s">
+      <c r="C65" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="D65" s="69"/>
-      <c r="E65" s="85" t="s">
+      <c r="D65" s="60"/>
+      <c r="E65" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="F65" s="72" t="s">
+      <c r="F65" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G65" s="70" t="s">
+      <c r="G65" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="H65" s="70">
-        <v>5</v>
-      </c>
-      <c r="I65" s="73"/>
-      <c r="J65" s="74">
+      <c r="H65" s="61">
+        <v>5</v>
+      </c>
+      <c r="I65" s="64"/>
+      <c r="J65" s="65">
         <v>42757</v>
       </c>
-      <c r="K65" s="70"/>
-      <c r="L65" s="71" t="s">
+      <c r="K65" s="61"/>
+      <c r="L65" s="62" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4183,7 +4174,7 @@
         <v>204</v>
       </c>
       <c r="D66" s="37"/>
-      <c r="E66" s="80" t="s">
+      <c r="E66" s="69" t="s">
         <v>205</v>
       </c>
       <c r="F66" s="7" t="s">
@@ -4210,10 +4201,10 @@
       <c r="C67" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D67" s="75" t="s">
+      <c r="D67" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E67" s="80"/>
+      <c r="E67" s="69"/>
       <c r="F67" s="54" t="s">
         <v>208</v>
       </c>
@@ -4243,7 +4234,7 @@
       <c r="D68" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="E68" s="86" t="s">
+      <c r="E68" s="75" t="s">
         <v>214</v>
       </c>
       <c r="F68" s="28" t="s">
@@ -4275,7 +4266,7 @@
       <c r="D69" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="E69" s="86"/>
+      <c r="E69" s="75"/>
       <c r="F69" s="28" t="s">
         <v>216</v>
       </c>
@@ -4305,7 +4296,7 @@
       <c r="D70" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="E70" s="80"/>
+      <c r="E70" s="69"/>
       <c r="F70" s="4" t="s">
         <v>215</v>
       </c>
@@ -4330,20 +4321,22 @@
         <v>8</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D71" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="E71" s="80"/>
-      <c r="F71" s="27" t="s">
+      <c r="D71" s="37">
+        <v>5</v>
+      </c>
+      <c r="E71" s="69" t="s">
         <v>218</v>
       </c>
+      <c r="F71" s="28" t="s">
+        <v>219</v>
+      </c>
       <c r="G71" s="4" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="H71" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="5">
@@ -4352,7 +4345,7 @@
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
     </row>
-    <row r="72" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
         <v>69</v>
       </c>
@@ -4360,20 +4353,22 @@
         <v>8</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D72" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="E72" s="80"/>
-      <c r="F72" s="27" t="s">
-        <v>219</v>
+      <c r="D72" s="37">
+        <v>7</v>
+      </c>
+      <c r="E72" s="69" t="s">
+        <v>220</v>
+      </c>
+      <c r="F72" s="28" t="s">
+        <v>234</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H72" s="4">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="H72" s="7">
+        <v>5</v>
       </c>
       <c r="I72" s="4"/>
       <c r="J72" s="5">
@@ -4390,14 +4385,12 @@
         <v>8</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D73" s="37">
-        <v>5</v>
-      </c>
-      <c r="E73" s="80" t="s">
-        <v>221</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E73" s="69"/>
       <c r="F73" s="28" t="s">
         <v>222</v>
       </c>
@@ -4418,25 +4411,25 @@
       <c r="A74" s="4">
         <v>71</v>
       </c>
-      <c r="B74" s="4">
-        <v>8</v>
+      <c r="B74" s="7">
+        <v>9</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D74" s="37">
-        <v>7</v>
-      </c>
-      <c r="E74" s="80" t="s">
-        <v>223</v>
+        <v>2</v>
+      </c>
+      <c r="E74" s="87" t="s">
+        <v>232</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H74" s="7">
+      <c r="H74" s="4">
         <v>5</v>
       </c>
       <c r="I74" s="4"/>
@@ -4450,17 +4443,17 @@
       <c r="A75" s="4">
         <v>72</v>
       </c>
-      <c r="B75" s="4">
-        <v>8</v>
+      <c r="B75" s="7">
+        <v>9</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D75" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="E75" s="80"/>
-      <c r="F75" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D75" s="37">
+        <v>3</v>
+      </c>
+      <c r="E75" s="88"/>
+      <c r="F75" s="28" t="s">
         <v>225</v>
       </c>
       <c r="G75" s="4" t="s">
@@ -4476,7 +4469,7 @@
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>73</v>
       </c>
@@ -4484,14 +4477,14 @@
         <v>9</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D76" s="37">
-        <v>1</v>
-      </c>
-      <c r="E76" s="80"/>
+        <v>4</v>
+      </c>
+      <c r="E76" s="69"/>
       <c r="F76" s="28" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>23</v>
@@ -4514,16 +4507,14 @@
         <v>9</v>
       </c>
       <c r="C77" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D77" s="37">
+        <v>5</v>
+      </c>
+      <c r="E77" s="69"/>
+      <c r="F77" s="28" t="s">
         <v>229</v>
-      </c>
-      <c r="D77" s="37">
-        <v>2</v>
-      </c>
-      <c r="E77" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F77" s="28" t="s">
-        <v>230</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>23</v>
@@ -4546,19 +4537,19 @@
         <v>9</v>
       </c>
       <c r="C78" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D78" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="D78" s="37">
-        <v>3</v>
-      </c>
-      <c r="E78" s="77"/>
+      <c r="E78" s="69"/>
       <c r="F78" s="28" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H78" s="4">
+      <c r="H78" s="7">
         <v>5</v>
       </c>
       <c r="I78" s="4"/>
@@ -4569,103 +4560,21 @@
       <c r="L78" s="4"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A79" s="4">
-        <v>76</v>
-      </c>
-      <c r="B79" s="7">
-        <v>9</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D79" s="37">
-        <v>4</v>
-      </c>
-      <c r="E79" s="80"/>
-      <c r="F79" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H79" s="4">
-        <v>5</v>
-      </c>
-      <c r="I79" s="4"/>
-      <c r="J79" s="5">
-        <v>42772</v>
-      </c>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="7"/>
+      <c r="D79" s="38"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" s="4">
-        <v>77</v>
-      </c>
-      <c r="B80" s="7">
-        <v>9</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D80" s="37">
-        <v>5</v>
-      </c>
-      <c r="E80" s="80"/>
-      <c r="F80" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H80" s="4">
-        <v>5</v>
-      </c>
-      <c r="I80" s="4"/>
-      <c r="J80" s="5">
-        <v>42772</v>
-      </c>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A81" s="4">
-        <v>78</v>
-      </c>
-      <c r="B81" s="7">
-        <v>9</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D81" s="37" t="s">
-        <v>236</v>
-      </c>
-      <c r="E81" s="80"/>
-      <c r="F81" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H81" s="7">
-        <v>5</v>
-      </c>
-      <c r="I81" s="4"/>
-      <c r="J81" s="5">
-        <v>42772</v>
-      </c>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D82" s="38"/>
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="L36:L45"/>
-    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E74:E75"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:I13">
     <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">

</xml_diff>

<commit_message>
Update bug log + test cases for iter 10
SD and mean for index not finalise
</commit_message>
<xml_diff>
--- a/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
+++ b/Documentation/Metrics/Bug Metrics/Bug Metrics.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="246">
   <si>
     <t>Task</t>
   </si>
@@ -688,9 +688,6 @@
     <t>Requirements changed for bootstrap (extra column).Data file not suitable</t>
   </si>
   <si>
-    <t>Bootstrap</t>
-  </si>
-  <si>
     <t>864 Records loaded</t>
   </si>
   <si>
@@ -703,9 +700,6 @@
     <t xml:space="preserve">No response when clicking the generated result button. Should display result </t>
   </si>
   <si>
-    <t>Partial resolved. Medical working but not VISA</t>
-  </si>
-  <si>
     <t>Report - KPI (VISA)</t>
   </si>
   <si>
@@ -782,13 +776,49 @@
   </si>
   <si>
     <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display only client age 0 - 2 for infant's screenings (age cap at 2 years old )  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">displayed age up till 77 years old which is incorrect </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenings - Infant  (View client list) </t>
+  </si>
+  <si>
+    <t>illness and screenings are not sorted in asc or desc order</t>
+  </si>
+  <si>
+    <t>Screenings - filter by gender ( view - adult)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenings - sort (view - adult and infant) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender = male , then display screenings for Male only </t>
+  </si>
+  <si>
+    <t xml:space="preserve">male selected, displayed both male and female which is incorrect </t>
+  </si>
+  <si>
+    <t>Client - Search</t>
+  </si>
+  <si>
+    <t>search "Sin" in search box, client name 'Lena Mardinis" appear</t>
+  </si>
+  <si>
+    <t>Upload / Bootstrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +872,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1016,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1173,7 +1211,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1244,6 +1281,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1720,7 +1761,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1773,7 +1814,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="78">
+      <c r="A3" s="77">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1800,7 +1841,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="78"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1825,7 +1866,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="78"/>
+      <c r="A5" s="77"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1850,7 +1891,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="78"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
@@ -1866,7 +1907,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="78"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1889,7 +1930,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="78"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1912,7 +1953,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="78"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
@@ -1937,7 +1978,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="78"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
@@ -1961,14 +2002,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="78"/>
-      <c r="B11" s="79" t="s">
+      <c r="A11" s="77"/>
+      <c r="B11" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="81"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -1979,7 +2020,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="82">
+      <c r="A12" s="81">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -2005,7 +2046,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="82"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
       </c>
@@ -2029,7 +2070,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="82"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="24" t="s">
         <v>46</v>
       </c>
@@ -2053,14 +2094,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="82"/>
-      <c r="B15" s="79" t="s">
+      <c r="A15" s="81"/>
+      <c r="B15" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="81"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -2068,7 +2109,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="77">
+      <c r="A16" s="76">
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -2092,14 +2133,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77" t="s">
+      <c r="A17" s="76"/>
+      <c r="B17" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -2107,11 +2148,11 @@
       <c r="H17" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="77">
+      <c r="A22" s="76">
         <v>8</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C22" s="46">
         <v>8</v>
@@ -2131,15 +2172,15 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="77"/>
+      <c r="A23" s="76"/>
       <c r="B23" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C23" s="46">
         <v>10</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E23" s="46">
         <v>2</v>
@@ -2153,14 +2194,14 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="77"/>
-      <c r="B24" s="77" t="s">
+      <c r="A24" s="76"/>
+      <c r="B24" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
       <c r="G24" s="13">
         <f>SUM(G22:G23)</f>
         <v>26</v>
@@ -2189,11 +2230,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2202,7 +2243,7 @@
     <col min="2" max="2" width="5.81640625" customWidth="1"/>
     <col min="3" max="3" width="36.1796875" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47" style="76" customWidth="1"/>
+    <col min="5" max="5" width="47" style="75" customWidth="1"/>
     <col min="6" max="6" width="38.54296875" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="10" max="10" width="12.81640625" customWidth="1"/>
@@ -2261,7 +2302,7 @@
       <c r="D2" s="48">
         <v>2</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="67" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="49" t="s">
@@ -2299,7 +2340,7 @@
       <c r="D3" s="48">
         <v>5</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="67" t="s">
         <v>38</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -2337,7 +2378,7 @@
       <c r="D4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="68" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="27" t="s">
@@ -2369,7 +2410,7 @@
       <c r="D5" s="37">
         <v>7</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="68" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="27" t="s">
@@ -2401,7 +2442,7 @@
       <c r="D6" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="68" t="s">
         <v>51</v>
       </c>
       <c r="F6" s="27" t="s">
@@ -2435,7 +2476,7 @@
       <c r="D7" s="37">
         <v>12</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="68" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="27" t="s">
@@ -2469,7 +2510,7 @@
       <c r="D8" s="37">
         <v>13</v>
       </c>
-      <c r="E8" s="69" t="s">
+      <c r="E8" s="68" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="27" t="s">
@@ -2501,7 +2542,7 @@
       <c r="D9" s="37">
         <v>14</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="68" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="27" t="s">
@@ -2533,7 +2574,7 @@
       <c r="D10" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="68" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="27" t="s">
@@ -2567,7 +2608,7 @@
       <c r="D11" s="37">
         <v>18</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="68" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="27" t="s">
@@ -2599,7 +2640,7 @@
       <c r="D12" s="37">
         <v>19</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E12" s="68" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="27" t="s">
@@ -2629,7 +2670,7 @@
       <c r="D13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="68" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="27" t="s">
@@ -2661,7 +2702,7 @@
       <c r="D14" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="68" t="s">
         <v>61</v>
       </c>
       <c r="F14" s="27" t="s">
@@ -2691,7 +2732,7 @@
       <c r="D15" s="38">
         <v>27</v>
       </c>
-      <c r="E15" s="69" t="s">
+      <c r="E15" s="68" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="31" t="s">
@@ -2723,7 +2764,7 @@
       <c r="D16" s="38">
         <v>28</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="69" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="31" t="s">
@@ -2757,7 +2798,7 @@
       <c r="D17" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="71" t="s">
+      <c r="E17" s="70" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="28" t="s">
@@ -2789,7 +2830,7 @@
       <c r="D18" s="37">
         <v>7</v>
       </c>
-      <c r="E18" s="71" t="s">
+      <c r="E18" s="70" t="s">
         <v>108</v>
       </c>
       <c r="F18" s="28" t="s">
@@ -2821,7 +2862,7 @@
       <c r="D19" s="37">
         <v>6</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="70" t="s">
         <v>76</v>
       </c>
       <c r="F19" s="28" t="s">
@@ -2853,7 +2894,7 @@
       <c r="D20" s="37">
         <v>8</v>
       </c>
-      <c r="E20" s="71" t="s">
+      <c r="E20" s="70" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="28" t="s">
@@ -2887,7 +2928,7 @@
       <c r="D21" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="71" t="s">
+      <c r="E21" s="70" t="s">
         <v>81</v>
       </c>
       <c r="F21" s="28" t="s">
@@ -2917,7 +2958,7 @@
         <v>82</v>
       </c>
       <c r="D22" s="41"/>
-      <c r="E22" s="72" t="s">
+      <c r="E22" s="71" t="s">
         <v>113</v>
       </c>
       <c r="F22" s="42" t="s">
@@ -2947,7 +2988,7 @@
         <v>82</v>
       </c>
       <c r="D23" s="41"/>
-      <c r="E23" s="72" t="s">
+      <c r="E23" s="71" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="42" t="s">
@@ -2975,7 +3016,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="41"/>
-      <c r="E24" s="72" t="s">
+      <c r="E24" s="71" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="42" t="s">
@@ -3005,7 +3046,7 @@
       <c r="D25" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="69" t="s">
         <v>116</v>
       </c>
       <c r="F25" s="33" t="s">
@@ -3039,7 +3080,7 @@
       <c r="D26" s="38">
         <v>30</v>
       </c>
-      <c r="E26" s="70" t="s">
+      <c r="E26" s="69" t="s">
         <v>136</v>
       </c>
       <c r="F26" s="35" t="s">
@@ -3064,10 +3105,10 @@
         <v>87</v>
       </c>
       <c r="D27" s="38"/>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="83"/>
+      <c r="F27" s="82"/>
     </row>
     <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
@@ -3078,7 +3119,7 @@
         <v>86</v>
       </c>
       <c r="D28" s="37"/>
-      <c r="E28" s="69" t="s">
+      <c r="E28" s="68" t="s">
         <v>88</v>
       </c>
       <c r="F28" s="28" t="s">
@@ -3102,7 +3143,7 @@
         <v>86</v>
       </c>
       <c r="D29" s="37"/>
-      <c r="E29" s="69" t="s">
+      <c r="E29" s="68" t="s">
         <v>89</v>
       </c>
       <c r="F29" s="28" t="s">
@@ -3124,7 +3165,7 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="37"/>
-      <c r="E30" s="69"/>
+      <c r="E30" s="68"/>
       <c r="F30" s="28" t="s">
         <v>101</v>
       </c>
@@ -3146,7 +3187,7 @@
         <v>70</v>
       </c>
       <c r="D31" s="37"/>
-      <c r="E31" s="69" t="s">
+      <c r="E31" s="68" t="s">
         <v>93</v>
       </c>
       <c r="F31" s="4"/>
@@ -3166,7 +3207,7 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="37"/>
-      <c r="E32" s="69" t="s">
+      <c r="E32" s="68" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="4"/>
@@ -3188,7 +3229,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="37"/>
-      <c r="E33" s="69" t="s">
+      <c r="E33" s="68" t="s">
         <v>95</v>
       </c>
       <c r="F33" s="4"/>
@@ -3210,7 +3251,7 @@
         <v>96</v>
       </c>
       <c r="D34" s="37"/>
-      <c r="E34" s="69" t="s">
+      <c r="E34" s="68" t="s">
         <v>97</v>
       </c>
       <c r="F34" s="4"/>
@@ -3268,12 +3309,12 @@
       <c r="H36" s="4">
         <v>1</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="84" t="s">
+      <c r="L36" s="83" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3302,12 +3343,12 @@
       <c r="H37" s="4">
         <v>5</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="85"/>
+      <c r="L37" s="84"/>
     </row>
     <row r="38" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
@@ -3334,12 +3375,12 @@
       <c r="H38" s="4">
         <v>5</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="85"/>
+      <c r="L38" s="84"/>
     </row>
     <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
@@ -3366,12 +3407,12 @@
       <c r="H39" s="4">
         <v>5</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="I39" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="85"/>
+      <c r="L39" s="84"/>
     </row>
     <row r="40" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
@@ -3398,12 +3439,12 @@
       <c r="H40" s="4">
         <v>5</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="85"/>
+      <c r="L40" s="84"/>
     </row>
     <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
@@ -3430,12 +3471,12 @@
       <c r="H41" s="4">
         <v>5</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="85"/>
+      <c r="L41" s="84"/>
     </row>
     <row r="42" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
@@ -3462,12 +3503,12 @@
       <c r="H42" s="4">
         <v>5</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="85"/>
+      <c r="L42" s="84"/>
     </row>
     <row r="43" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
@@ -3494,12 +3535,12 @@
       <c r="H43" s="4">
         <v>5</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="85"/>
+      <c r="L43" s="84"/>
     </row>
     <row r="44" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
@@ -3526,12 +3567,12 @@
       <c r="H44" s="4">
         <v>5</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="85"/>
+      <c r="L44" s="84"/>
     </row>
     <row r="45" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
@@ -3554,14 +3595,14 @@
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="4" t="s">
+      <c r="I45" s="88" t="s">
         <v>42</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="5">
         <v>42757</v>
       </c>
-      <c r="L45" s="86"/>
+      <c r="L45" s="85"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
@@ -3706,7 +3747,7 @@
         <v>164</v>
       </c>
       <c r="D50" s="37"/>
-      <c r="E50" s="73" t="s">
+      <c r="E50" s="72" t="s">
         <v>163</v>
       </c>
       <c r="F50" s="57" t="s">
@@ -3790,7 +3831,7 @@
         <v>170</v>
       </c>
       <c r="D53" s="37"/>
-      <c r="E53" s="69"/>
+      <c r="E53" s="68"/>
       <c r="F53" s="54" t="s">
         <v>171</v>
       </c>
@@ -3820,7 +3861,7 @@
         <v>170</v>
       </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="69"/>
+      <c r="E54" s="68"/>
       <c r="F54" s="54" t="s">
         <v>173</v>
       </c>
@@ -3850,7 +3891,7 @@
         <v>170</v>
       </c>
       <c r="D55" s="37"/>
-      <c r="E55" s="69"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="54" t="s">
         <v>172</v>
       </c>
@@ -3880,7 +3921,7 @@
         <v>174</v>
       </c>
       <c r="D56" s="37"/>
-      <c r="E56" s="69"/>
+      <c r="E56" s="68"/>
       <c r="F56" s="54" t="s">
         <v>175</v>
       </c>
@@ -3910,7 +3951,7 @@
         <v>193</v>
       </c>
       <c r="D57" s="37"/>
-      <c r="E57" s="69"/>
+      <c r="E57" s="68"/>
       <c r="F57" s="54" t="s">
         <v>195</v>
       </c>
@@ -3936,7 +3977,7 @@
         <v>176</v>
       </c>
       <c r="D58" s="37"/>
-      <c r="E58" s="69" t="s">
+      <c r="E58" s="68" t="s">
         <v>177</v>
       </c>
       <c r="F58" s="54" t="s">
@@ -3968,7 +4009,7 @@
         <v>179</v>
       </c>
       <c r="D59" s="37"/>
-      <c r="E59" s="69" t="s">
+      <c r="E59" s="68" t="s">
         <v>182</v>
       </c>
       <c r="F59" s="54" t="s">
@@ -3998,7 +4039,7 @@
         <v>181</v>
       </c>
       <c r="D60" s="55"/>
-      <c r="E60" s="69" t="s">
+      <c r="E60" s="68" t="s">
         <v>183</v>
       </c>
       <c r="F60" s="4"/>
@@ -4028,7 +4069,7 @@
         <v>170</v>
       </c>
       <c r="D61" s="55"/>
-      <c r="E61" s="69" t="s">
+      <c r="E61" s="68" t="s">
         <v>191</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -4089,7 +4130,7 @@
       <c r="E63" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="F63" s="67" t="s">
+      <c r="F63" s="66" t="s">
         <v>200</v>
       </c>
       <c r="G63" s="4" t="s">
@@ -4144,7 +4185,7 @@
         <v>184</v>
       </c>
       <c r="D65" s="60"/>
-      <c r="E65" s="74" t="s">
+      <c r="E65" s="73" t="s">
         <v>185</v>
       </c>
       <c r="F65" s="63" t="s">
@@ -4156,14 +4197,16 @@
       <c r="H65" s="61">
         <v>5</v>
       </c>
-      <c r="I65" s="64"/>
-      <c r="J65" s="65">
+      <c r="I65" s="89" t="s">
+        <v>138</v>
+      </c>
+      <c r="J65" s="64">
         <v>42757</v>
       </c>
-      <c r="K65" s="61"/>
-      <c r="L65" s="62" t="s">
-        <v>209</v>
-      </c>
+      <c r="K65" s="64">
+        <v>42774</v>
+      </c>
+      <c r="L65" s="62"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
@@ -4171,14 +4214,14 @@
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" s="37"/>
+      <c r="E66" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="D66" s="37"/>
-      <c r="E66" s="69" t="s">
+      <c r="F66" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>23</v>
@@ -4186,9 +4229,13 @@
       <c r="H66" s="7">
         <v>5</v>
       </c>
-      <c r="I66" s="4"/>
+      <c r="I66" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
+      <c r="K66" s="64">
+        <v>42774</v>
+      </c>
       <c r="L66" s="4"/>
     </row>
     <row r="67" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -4199,14 +4246,14 @@
         <v>8</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D67" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="D67" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="E67" s="69"/>
+      <c r="E67" s="68"/>
       <c r="F67" s="54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>23</v>
@@ -4214,11 +4261,15 @@
       <c r="H67" s="4">
         <v>5</v>
       </c>
-      <c r="I67" s="4"/>
+      <c r="I67" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="J67" s="5">
         <v>42772</v>
       </c>
-      <c r="K67" s="4"/>
+      <c r="K67" s="64">
+        <v>42774</v>
+      </c>
       <c r="L67" s="4"/>
     </row>
     <row r="68" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -4229,16 +4280,16 @@
         <v>8</v>
       </c>
       <c r="C68" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="F68" s="28" t="s">
         <v>211</v>
-      </c>
-      <c r="D68" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="E68" s="75" t="s">
-        <v>214</v>
-      </c>
-      <c r="F68" s="28" t="s">
-        <v>213</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>23</v>
@@ -4261,14 +4312,14 @@
         <v>8</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D69" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="E69" s="75"/>
+        <v>210</v>
+      </c>
+      <c r="E69" s="74"/>
       <c r="F69" s="28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>50</v>
@@ -4291,14 +4342,14 @@
         <v>8</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D70" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="E70" s="69"/>
+        <v>210</v>
+      </c>
+      <c r="E70" s="68"/>
       <c r="F70" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>23</v>
@@ -4321,16 +4372,16 @@
         <v>8</v>
       </c>
       <c r="C71" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D71" s="37">
+        <v>5</v>
+      </c>
+      <c r="E71" s="68" t="s">
+        <v>216</v>
+      </c>
+      <c r="F71" s="28" t="s">
         <v>217</v>
-      </c>
-      <c r="D71" s="37">
-        <v>5</v>
-      </c>
-      <c r="E71" s="69" t="s">
-        <v>218</v>
-      </c>
-      <c r="F71" s="28" t="s">
-        <v>219</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>23</v>
@@ -4353,16 +4404,16 @@
         <v>8</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D72" s="37">
         <v>7</v>
       </c>
-      <c r="E72" s="69" t="s">
-        <v>220</v>
+      <c r="E72" s="68" t="s">
+        <v>218</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>23</v>
@@ -4385,14 +4436,14 @@
         <v>8</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D73" s="37">
         <v>1</v>
       </c>
-      <c r="E73" s="69"/>
+      <c r="E73" s="68"/>
       <c r="F73" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>23</v>
@@ -4415,16 +4466,16 @@
         <v>9</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D74" s="37">
         <v>2</v>
       </c>
-      <c r="E74" s="87" t="s">
-        <v>232</v>
+      <c r="E74" s="86" t="s">
+        <v>230</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>23</v>
@@ -4447,14 +4498,14 @@
         <v>9</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D75" s="37">
         <v>3</v>
       </c>
-      <c r="E75" s="88"/>
+      <c r="E75" s="87"/>
       <c r="F75" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>23</v>
@@ -4477,14 +4528,14 @@
         <v>9</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D76" s="37">
         <v>4</v>
       </c>
-      <c r="E76" s="69"/>
+      <c r="E76" s="68"/>
       <c r="F76" s="28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>23</v>
@@ -4507,14 +4558,14 @@
         <v>9</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D77" s="37">
         <v>5</v>
       </c>
-      <c r="E77" s="69"/>
+      <c r="E77" s="68"/>
       <c r="F77" s="28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>23</v>
@@ -4537,19 +4588,19 @@
         <v>9</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D78" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="E78" s="68"/>
+      <c r="F78" s="28" t="s">
         <v>231</v>
-      </c>
-      <c r="E78" s="69"/>
-      <c r="F78" s="28" t="s">
-        <v>233</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H78" s="7">
+      <c r="H78" s="4">
         <v>5</v>
       </c>
       <c r="I78" s="4"/>
@@ -4559,16 +4610,133 @@
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A79" s="4"/>
-      <c r="B79" s="7"/>
-      <c r="D79" s="38"/>
+    <row r="79" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="4">
+        <v>76</v>
+      </c>
+      <c r="B79" s="7">
+        <v>7</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D79" s="37"/>
+      <c r="E79" s="68" t="s">
+        <v>234</v>
+      </c>
+      <c r="F79" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H79" s="4">
+        <v>5</v>
+      </c>
+      <c r="I79" s="4"/>
+      <c r="J79" s="5">
+        <v>42774</v>
+      </c>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" s="4"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="4"/>
+      <c r="A80" s="4">
+        <v>77</v>
+      </c>
+      <c r="B80" s="7">
+        <v>7</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="68"/>
+      <c r="F80" s="68" t="s">
+        <v>237</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="5">
+        <v>42774</v>
+      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+    </row>
+    <row r="81" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="4">
+        <v>78</v>
+      </c>
+      <c r="B81" s="7">
+        <v>7</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="68" t="s">
+        <v>240</v>
+      </c>
+      <c r="F81" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H81" s="4">
+        <v>5</v>
+      </c>
+      <c r="I81" s="4"/>
+      <c r="J81" s="5">
+        <v>42774</v>
+      </c>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+    </row>
+    <row r="82" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="4">
+        <v>79</v>
+      </c>
+      <c r="B82" s="7">
+        <v>7</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D82" s="4"/>
+      <c r="E82" s="68"/>
+      <c r="F82" s="53" t="s">
+        <v>243</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H82" s="4">
+        <v>5</v>
+      </c>
+      <c r="I82" s="4"/>
+      <c r="J82" s="5">
+        <v>42774</v>
+      </c>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="68"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>